<commit_message>
Change filter.farm to filter.lease_area in DDSs and change cable landing points table to project.site
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -1455,9 +1455,6 @@
     <t>reference.view_component_collection_point</t>
   </si>
   <si>
-    <t>filter.farm</t>
-  </si>
-  <si>
     <t>filter.cable_corridor</t>
   </si>
   <si>
@@ -1492,6 +1489,9 @@
   </si>
   <si>
     <t>reference.equipment_soil_lay_rates</t>
+  </si>
+  <si>
+    <t>filter.lease_area</t>
   </si>
 </sst>
 </file>
@@ -6370,7 +6370,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>267</v>
@@ -6438,7 +6438,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>267</v>
@@ -6507,7 +6507,7 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>267</v>
@@ -6575,7 +6575,7 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>267</v>
@@ -6631,7 +6631,7 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>317</v>
@@ -6696,7 +6696,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>267</v>
@@ -6764,7 +6764,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>267</v>
@@ -6826,7 +6826,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="C12" t="s">
         <v>333</v>
@@ -6837,7 +6837,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="C13" t="s">
         <v>334</v>
@@ -6848,7 +6848,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C14" t="s">
         <v>333</v>
@@ -6859,7 +6859,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C15" t="s">
         <v>334</v>
@@ -6870,7 +6870,7 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C16" t="s">
         <v>335</v>
@@ -6881,7 +6881,7 @@
         <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C17" t="s">
         <v>336</v>
@@ -6892,7 +6892,7 @@
         <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C18" t="s">
         <v>337</v>
@@ -6925,7 +6925,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C21" t="s">
         <v>340</v>
@@ -6983,7 +6983,7 @@
         <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="C23" t="s">
         <v>335</v>
@@ -6994,7 +6994,7 @@
         <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="C24" t="s">
         <v>337</v>
@@ -7005,7 +7005,7 @@
         <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="C25" t="s">
         <v>354</v>
@@ -7016,7 +7016,7 @@
         <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C26" t="s">
         <v>355</v>
@@ -7094,7 +7094,7 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C32" t="s">
         <v>363</v>
@@ -7105,7 +7105,7 @@
         <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C33" t="s">
         <v>355</v>

</xml_diff>

<commit_message>
Change identifiers bathymetry.max_soil_resistivity and bathymetry.max_seabed_temp to farm.max_soil_resistivity and farm.max_seabed_temp
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="318" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="318"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">ROOT!$A$1:$H$45</definedName>
     <definedName name="A">ROOT!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="490">
   <si>
     <t>Identifier</t>
   </si>
@@ -1492,19 +1492,32 @@
   </si>
   <si>
     <t>filter.lease_area</t>
+  </si>
+  <si>
+    <t>farm.max_soil_resistivity</t>
+  </si>
+  <si>
+    <t>farm.max_seabed_temp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1615,27 +1628,27 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1643,7 +1656,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1651,14 +1664,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1670,19 +1683,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -2063,9 +2077,9 @@
   </sheetPr>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C58" sqref="C58"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2108,8 +2122,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
-        <v>6</v>
+      <c r="A2" s="37" t="s">
+        <v>488</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>7</v>
@@ -2128,8 +2142,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="30" t="s">
-        <v>10</v>
+      <c r="A3" s="37" t="s">
+        <v>489</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>7</v>
@@ -6185,7 +6199,7 @@
   </sheetPr>
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change units of environmental directions in cable corridor to degrees from radians
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="318"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="318" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="489">
   <si>
     <t>Identifier</t>
   </si>
@@ -784,9 +784,6 @@
   </si>
   <si>
     <t>Var</t>
-  </si>
-  <si>
-    <t>degree</t>
   </si>
   <si>
     <t>K.m/W</t>
@@ -2077,7 +2074,7 @@
   </sheetPr>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -2109,10 +2106,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>471</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>472</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -2123,16 +2120,16 @@
     </row>
     <row r="2" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="37" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="30" t="s">
+        <v>377</v>
+      </c>
+      <c r="D2" s="31" t="s">
         <v>378</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>379</v>
       </c>
       <c r="G2" s="32" t="s">
         <v>8</v>
@@ -2143,16 +2140,16 @@
     </row>
     <row r="3" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="37" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="30" t="s">
+        <v>379</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>380</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>381</v>
       </c>
       <c r="G3" s="32" t="s">
         <v>8</v>
@@ -2169,10 +2166,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>382</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>383</v>
       </c>
       <c r="G4" s="32" t="s">
         <v>8</v>
@@ -2189,10 +2186,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="30" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5" s="31" t="s">
         <v>384</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>385</v>
       </c>
       <c r="G5" s="32" t="s">
         <v>8</v>
@@ -2212,7 +2209,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H6" s="30" t="s">
         <v>9</v>
@@ -2229,7 +2226,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H7" s="30" t="s">
         <v>9</v>
@@ -2246,7 +2243,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H8" s="30" t="s">
         <v>9</v>
@@ -2260,10 +2257,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>389</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>390</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>14</v>
@@ -2297,7 +2294,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H11" s="30" t="s">
         <v>9</v>
@@ -2314,7 +2311,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H12" s="30" t="s">
         <v>9</v>
@@ -2331,7 +2328,7 @@
         <v>32</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H13" s="30" t="s">
         <v>9</v>
@@ -2348,7 +2345,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H14" s="30" t="s">
         <v>9</v>
@@ -2365,7 +2362,7 @@
         <v>36</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H15" s="30" t="s">
         <v>9</v>
@@ -2379,10 +2376,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>396</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>397</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>14</v>
@@ -2396,10 +2393,10 @@
         <v>39</v>
       </c>
       <c r="C17" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="D17" s="31" t="s">
         <v>398</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>399</v>
       </c>
       <c r="G17" s="30" t="s">
         <v>8</v>
@@ -2416,10 +2413,10 @@
         <v>41</v>
       </c>
       <c r="C18" s="30" t="s">
+        <v>373</v>
+      </c>
+      <c r="D18" s="31" t="s">
         <v>374</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>375</v>
       </c>
       <c r="H18" s="30" t="s">
         <v>9</v>
@@ -2433,10 +2430,10 @@
         <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>400</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>401</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>14</v>
@@ -2450,10 +2447,10 @@
         <v>7</v>
       </c>
       <c r="C20" s="30" t="s">
+        <v>375</v>
+      </c>
+      <c r="D20" s="31" t="s">
         <v>376</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>377</v>
       </c>
       <c r="G20" s="30" t="s">
         <v>8</v>
@@ -2470,10 +2467,10 @@
         <v>7</v>
       </c>
       <c r="C21" s="30" t="s">
+        <v>401</v>
+      </c>
+      <c r="D21" s="31" t="s">
         <v>402</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>403</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>8</v>
@@ -2490,10 +2487,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="D22" s="31" t="s">
         <v>404</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>405</v>
       </c>
       <c r="G22" s="30" t="s">
         <v>8</v>
@@ -2504,16 +2501,16 @@
     </row>
     <row r="23" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="30" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="30" t="s">
+        <v>455</v>
+      </c>
+      <c r="D23" s="31" t="s">
         <v>456</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>457</v>
       </c>
       <c r="G23" s="30" t="s">
         <v>46</v>
@@ -2530,10 +2527,10 @@
         <v>7</v>
       </c>
       <c r="C24" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="D24" s="31" t="s">
         <v>406</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>407</v>
       </c>
       <c r="G24" s="30" t="s">
         <v>46</v>
@@ -2553,7 +2550,7 @@
         <v>49</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>14</v>
@@ -2567,7 +2564,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D26" s="34" t="s">
         <v>51</v>
@@ -2587,7 +2584,7 @@
         <v>54</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>14</v>
@@ -2604,7 +2601,7 @@
         <v>56</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>14</v>
@@ -2621,7 +2618,7 @@
         <v>58</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>14</v>
@@ -2635,10 +2632,10 @@
         <v>13</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>413</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>414</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>14</v>
@@ -2672,10 +2669,10 @@
         <v>64</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>415</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>416</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -2692,7 +2689,7 @@
         <v>41</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D33" s="35" t="s">
         <v>66</v>
@@ -2714,10 +2711,10 @@
         <v>13</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>418</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>419</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>8</v>
@@ -2737,7 +2734,7 @@
         <v>69</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2757,7 +2754,7 @@
         <v>71</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -2777,7 +2774,7 @@
         <v>73</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>14</v>
@@ -2794,7 +2791,7 @@
         <v>75</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>14</v>
@@ -2811,7 +2808,7 @@
         <v>78</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>52</v>
@@ -2828,7 +2825,7 @@
         <v>81</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>52</v>
@@ -2845,7 +2842,7 @@
         <v>83</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>52</v>
@@ -2859,10 +2856,10 @@
         <v>80</v>
       </c>
       <c r="C42" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="D42" s="26" t="s">
         <v>427</v>
-      </c>
-      <c r="D42" s="26" t="s">
-        <v>428</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>52</v>
@@ -2879,7 +2876,7 @@
         <v>17</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>52</v>
@@ -2913,10 +2910,10 @@
         <v>90</v>
       </c>
       <c r="C45" s="30" t="s">
+        <v>429</v>
+      </c>
+      <c r="D45" s="31" t="s">
         <v>430</v>
-      </c>
-      <c r="D45" s="31" t="s">
-        <v>431</v>
       </c>
       <c r="G45" s="30" t="s">
         <v>46</v>
@@ -2933,10 +2930,10 @@
         <v>92</v>
       </c>
       <c r="C46" s="30" t="s">
+        <v>431</v>
+      </c>
+      <c r="D46" s="31" t="s">
         <v>432</v>
-      </c>
-      <c r="D46" s="31" t="s">
-        <v>433</v>
       </c>
       <c r="G46" s="30" t="s">
         <v>46</v>
@@ -2953,10 +2950,10 @@
         <v>7</v>
       </c>
       <c r="C47" s="30" t="s">
+        <v>433</v>
+      </c>
+      <c r="D47" s="31" t="s">
         <v>434</v>
-      </c>
-      <c r="D47" s="31" t="s">
-        <v>435</v>
       </c>
       <c r="G47" s="30" t="s">
         <v>46</v>
@@ -2973,10 +2970,10 @@
         <v>80</v>
       </c>
       <c r="C48" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="D48" s="26" t="s">
         <v>436</v>
-      </c>
-      <c r="D48" s="26" t="s">
-        <v>437</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>52</v>
@@ -2990,10 +2987,10 @@
         <v>96</v>
       </c>
       <c r="C49" s="30" t="s">
+        <v>437</v>
+      </c>
+      <c r="D49" s="31" t="s">
         <v>438</v>
-      </c>
-      <c r="D49" s="31" t="s">
-        <v>439</v>
       </c>
       <c r="G49" s="30" t="s">
         <v>46</v>
@@ -3010,10 +3007,10 @@
         <v>13</v>
       </c>
       <c r="C50" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="D50" s="27" t="s">
         <v>440</v>
-      </c>
-      <c r="D50" s="27" t="s">
-        <v>441</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="7" t="s">
@@ -3028,10 +3025,10 @@
         <v>7</v>
       </c>
       <c r="C51" s="30" t="s">
+        <v>441</v>
+      </c>
+      <c r="D51" s="31" t="s">
         <v>442</v>
-      </c>
-      <c r="D51" s="31" t="s">
-        <v>443</v>
       </c>
       <c r="G51" s="30" t="s">
         <v>8</v>
@@ -3051,7 +3048,7 @@
         <v>100</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G52" s="30" t="s">
         <v>8</v>
@@ -3071,7 +3068,7 @@
         <v>102</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G53" s="30" t="s">
         <v>8</v>
@@ -3085,10 +3082,10 @@
         <v>90</v>
       </c>
       <c r="C54" s="30" t="s">
+        <v>451</v>
+      </c>
+      <c r="D54" s="31" t="s">
         <v>452</v>
-      </c>
-      <c r="D54" s="31" t="s">
-        <v>453</v>
       </c>
       <c r="G54" s="30" t="s">
         <v>46</v>
@@ -3105,7 +3102,7 @@
         <v>105</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G55" s="30" t="s">
         <v>46</v>
@@ -3179,10 +3176,10 @@
         <v>107</v>
       </c>
       <c r="C59" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="D59" s="28" t="s">
         <v>450</v>
-      </c>
-      <c r="D59" s="28" t="s">
-        <v>451</v>
       </c>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
@@ -3199,10 +3196,10 @@
         <v>120</v>
       </c>
       <c r="C60" s="30" t="s">
+        <v>445</v>
+      </c>
+      <c r="D60" s="31" t="s">
         <v>446</v>
-      </c>
-      <c r="D60" s="31" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -3213,24 +3210,24 @@
         <v>122</v>
       </c>
       <c r="C61" s="30" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="33" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B62" s="33" t="s">
         <v>13</v>
       </c>
       <c r="C62" s="33" t="s">
+        <v>462</v>
+      </c>
+      <c r="D62" s="34" t="s">
         <v>463</v>
-      </c>
-      <c r="D62" s="34" t="s">
-        <v>464</v>
       </c>
       <c r="H62" s="33" t="s">
         <v>14</v>
@@ -3238,16 +3235,16 @@
     </row>
     <row r="63" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="33" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B63" s="33" t="s">
         <v>13</v>
       </c>
       <c r="C63" s="33" t="s">
+        <v>465</v>
+      </c>
+      <c r="D63" s="34" t="s">
         <v>466</v>
-      </c>
-      <c r="D63" s="34" t="s">
-        <v>467</v>
       </c>
       <c r="H63" s="33" t="s">
         <v>52</v>
@@ -3255,16 +3252,16 @@
     </row>
     <row r="64" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="33" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B64" s="33" t="s">
         <v>13</v>
       </c>
       <c r="C64" s="33" t="s">
+        <v>468</v>
+      </c>
+      <c r="D64" s="34" t="s">
         <v>469</v>
-      </c>
-      <c r="D64" s="34" t="s">
-        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -3900,7 +3897,7 @@
         <v>139</v>
       </c>
       <c r="H12" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I12" t="s">
         <v>190</v>
@@ -5166,7 +5163,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="21" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B49" s="21" t="s">
         <v>223</v>
@@ -5188,7 +5185,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="20" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B50" t="s">
         <v>223</v>
@@ -5196,7 +5193,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="20" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B51" t="s">
         <v>223</v>
@@ -5204,7 +5201,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="20" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B52" t="s">
         <v>222</v>
@@ -5223,8 +5220,8 @@
   </sheetPr>
   <dimension ref="A1:AE45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5782,7 +5779,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
@@ -5790,7 +5787,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.35">
@@ -5801,10 +5798,10 @@
         <v>248</v>
       </c>
       <c r="C12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.35">
@@ -5812,7 +5809,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.35">
@@ -5820,7 +5817,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.35">
@@ -5828,7 +5825,7 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.35">
@@ -5836,7 +5833,7 @@
         <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
@@ -5844,7 +5841,7 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
@@ -5855,10 +5852,10 @@
         <v>248</v>
       </c>
       <c r="C18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
@@ -5874,7 +5871,7 @@
         <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C20" t="s">
         <v>225</v>
@@ -5893,7 +5890,7 @@
         <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
@@ -5901,7 +5898,7 @@
         <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
@@ -5909,10 +5906,10 @@
         <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
@@ -5969,7 +5966,7 @@
         <v>243</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F30" t="s">
         <v>239</v>
@@ -6019,7 +6016,7 @@
         <v>243</v>
       </c>
       <c r="E31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F31" t="s">
         <v>239</v>
@@ -6045,7 +6042,7 @@
         <v>98</v>
       </c>
       <c r="B33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -6053,7 +6050,7 @@
         <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -6061,7 +6058,7 @@
         <v>101</v>
       </c>
       <c r="B35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -6172,7 +6169,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="20" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B44" t="s">
         <v>225</v>
@@ -6180,7 +6177,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="20" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B45" t="s">
         <v>225</v>
@@ -6245,16 +6242,16 @@
         <v>217</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>263</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>264</v>
       </c>
       <c r="F1" s="2"/>
     </row>
@@ -6263,10 +6260,10 @@
         <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.35">
@@ -6274,10 +6271,10 @@
         <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.35">
@@ -6285,97 +6282,97 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" t="s">
         <v>272</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>273</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="L4" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="M4" t="s">
         <v>276</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>277</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>278</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>279</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>280</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>281</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>282</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" t="s">
         <v>284</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>285</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>286</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>287</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>288</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="Z4" s="20" t="s">
+      <c r="AA4" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="AA4" s="20" t="s">
+      <c r="AB4" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="AB4" s="20" t="s">
+      <c r="AC4" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="AC4" s="20" t="s">
+      <c r="AD4" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="AD4" s="20" t="s">
+      <c r="AE4" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="AG4" s="1"/>
     </row>
@@ -6384,67 +6381,67 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I5" t="s">
+        <v>277</v>
+      </c>
+      <c r="J5" t="s">
+        <v>278</v>
+      </c>
+      <c r="K5" t="s">
         <v>299</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="I5" t="s">
-        <v>278</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
+        <v>300</v>
+      </c>
+      <c r="M5" t="s">
         <v>279</v>
       </c>
-      <c r="K5" t="s">
-        <v>300</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
+        <v>280</v>
+      </c>
+      <c r="O5" t="s">
+        <v>285</v>
+      </c>
+      <c r="P5" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q5" t="s">
         <v>301</v>
       </c>
-      <c r="M5" t="s">
-        <v>280</v>
-      </c>
-      <c r="N5" t="s">
-        <v>281</v>
-      </c>
-      <c r="O5" t="s">
-        <v>286</v>
-      </c>
-      <c r="P5" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>302</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="T5" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="T5" s="20" t="s">
-        <v>305</v>
-      </c>
       <c r="U5" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.35">
@@ -6452,67 +6449,67 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" t="s">
         <v>309</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>310</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>311</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>312</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
+        <v>279</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="P6" t="s">
         <v>313</v>
       </c>
-      <c r="M6" t="s">
-        <v>280</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>314</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>315</v>
       </c>
-      <c r="R6" t="s">
-        <v>316</v>
-      </c>
       <c r="S6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="U6" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="W6" s="1"/>
     </row>
@@ -6521,67 +6518,67 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" t="s">
         <v>309</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>310</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>311</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>312</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
+        <v>279</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="P7" t="s">
         <v>313</v>
       </c>
-      <c r="M7" t="s">
-        <v>280</v>
-      </c>
-      <c r="N7" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="O7" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>314</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>315</v>
       </c>
-      <c r="R7" t="s">
-        <v>316</v>
-      </c>
       <c r="S7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="U7" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="V7" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.35">
@@ -6589,52 +6586,52 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="F8" s="20" t="s">
-        <v>275</v>
-      </c>
       <c r="G8" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" t="s">
         <v>278</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
+        <v>284</v>
+      </c>
+      <c r="K8" t="s">
+        <v>286</v>
+      </c>
+      <c r="L8" t="s">
+        <v>280</v>
+      </c>
+      <c r="M8" t="s">
         <v>279</v>
       </c>
-      <c r="J8" t="s">
-        <v>285</v>
-      </c>
-      <c r="K8" t="s">
-        <v>287</v>
-      </c>
-      <c r="L8" t="s">
-        <v>281</v>
-      </c>
-      <c r="M8" t="s">
-        <v>280</v>
-      </c>
       <c r="N8" t="s">
+        <v>301</v>
+      </c>
+      <c r="O8" t="s">
         <v>302</v>
       </c>
-      <c r="O8" t="s">
-        <v>303</v>
-      </c>
       <c r="P8" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
@@ -6645,64 +6642,64 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="J9" t="s">
         <v>322</v>
       </c>
-      <c r="I9" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>323</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>324</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
+        <v>279</v>
+      </c>
+      <c r="N9" t="s">
+        <v>280</v>
+      </c>
+      <c r="O9" t="s">
+        <v>283</v>
+      </c>
+      <c r="P9" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>301</v>
+      </c>
+      <c r="R9" t="s">
+        <v>302</v>
+      </c>
+      <c r="S9" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="M9" t="s">
-        <v>280</v>
-      </c>
-      <c r="N9" t="s">
-        <v>281</v>
-      </c>
-      <c r="O9" t="s">
-        <v>284</v>
-      </c>
-      <c r="P9" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>302</v>
-      </c>
-      <c r="R9" t="s">
-        <v>303</v>
-      </c>
-      <c r="S9" s="20" t="s">
-        <v>326</v>
-      </c>
       <c r="T9" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="U9" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.35">
@@ -6710,67 +6707,67 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I10" t="s">
+        <v>277</v>
+      </c>
+      <c r="J10" t="s">
+        <v>278</v>
+      </c>
+      <c r="K10" t="s">
         <v>299</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="I10" t="s">
-        <v>278</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
+        <v>300</v>
+      </c>
+      <c r="M10" t="s">
         <v>279</v>
       </c>
-      <c r="K10" t="s">
-        <v>300</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
+        <v>280</v>
+      </c>
+      <c r="O10" t="s">
+        <v>285</v>
+      </c>
+      <c r="P10" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q10" t="s">
         <v>301</v>
       </c>
-      <c r="M10" t="s">
-        <v>280</v>
-      </c>
-      <c r="N10" t="s">
-        <v>281</v>
-      </c>
-      <c r="O10" t="s">
-        <v>286</v>
-      </c>
-      <c r="P10" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>302</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="S10" s="20" t="s">
+      <c r="T10" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="T10" s="20" t="s">
-        <v>305</v>
-      </c>
       <c r="U10" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="V10" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.35">
@@ -6778,61 +6775,61 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E11" t="s">
+        <v>326</v>
+      </c>
+      <c r="F11" t="s">
         <v>327</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>328</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="I11" t="s">
+        <v>286</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="H11" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="I11" t="s">
-        <v>287</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" t="s">
         <v>331</v>
       </c>
-      <c r="L11" t="s">
-        <v>332</v>
-      </c>
       <c r="M11" t="s">
+        <v>283</v>
+      </c>
+      <c r="N11" t="s">
+        <v>280</v>
+      </c>
+      <c r="O11" t="s">
+        <v>279</v>
+      </c>
+      <c r="P11" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>302</v>
+      </c>
+      <c r="R11" t="s">
         <v>284</v>
       </c>
-      <c r="N11" t="s">
-        <v>281</v>
-      </c>
-      <c r="O11" t="s">
-        <v>280</v>
-      </c>
-      <c r="P11" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>303</v>
-      </c>
-      <c r="R11" t="s">
-        <v>285</v>
-      </c>
       <c r="S11" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.35">
@@ -6840,10 +6837,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
@@ -6851,10 +6848,10 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.35">
@@ -6862,10 +6859,10 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.35">
@@ -6873,10 +6870,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.35">
@@ -6884,10 +6881,10 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -6895,10 +6892,10 @@
         <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
@@ -6906,10 +6903,10 @@
         <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
@@ -6917,10 +6914,10 @@
         <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
@@ -6928,10 +6925,10 @@
         <v>95</v>
       </c>
       <c r="B20" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
@@ -6939,46 +6936,46 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C21" t="s">
+        <v>339</v>
+      </c>
+      <c r="D21" t="s">
         <v>340</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>341</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>342</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>343</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>344</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>345</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>346</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>347</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>348</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>349</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>350</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>351</v>
-      </c>
-      <c r="O21" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
@@ -6986,10 +6983,10 @@
         <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
@@ -6997,10 +6994,10 @@
         <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C23" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
@@ -7008,10 +7005,10 @@
         <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
@@ -7019,10 +7016,10 @@
         <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
@@ -7030,16 +7027,16 @@
         <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C26" t="s">
+        <v>354</v>
+      </c>
+      <c r="D26" t="s">
         <v>355</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>356</v>
-      </c>
-      <c r="E26" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
@@ -7047,10 +7044,10 @@
         <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
@@ -7058,10 +7055,10 @@
         <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
@@ -7069,10 +7066,10 @@
         <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
@@ -7080,13 +7077,13 @@
         <v>119</v>
       </c>
       <c r="B30" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
@@ -7094,13 +7091,13 @@
         <v>121</v>
       </c>
       <c r="B31" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
@@ -7108,10 +7105,10 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
@@ -7119,27 +7116,27 @@
         <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C33" t="s">
+        <v>354</v>
+      </c>
+      <c r="D33" t="s">
         <v>355</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>356</v>
-      </c>
-      <c r="E33" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="23" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
@@ -7184,16 +7181,16 @@
         <v>217</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>366</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -7201,10 +7198,10 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C2" t="s">
         <v>368</v>
-      </c>
-      <c r="C2" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -7212,46 +7209,46 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C3" t="s">
         <v>370</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>371</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>372</v>
-      </c>
-      <c r="E3" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>458</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>459</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>460</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B5" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>370</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="D5" s="24" t="s">
         <v>371</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="E5" s="24" t="s">
         <v>372</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DDS variable name changes and description updates
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -1446,15 +1446,9 @@
     <t>filter.cable_corridor</t>
   </si>
   <si>
-    <t>filter.constraint_activity_frequency</t>
-  </si>
-  <si>
     <t>filter.cable_corridor_constraint</t>
   </si>
   <si>
-    <t>filter.cable_corridor_constraint_activity_frequency</t>
-  </si>
-  <si>
     <t>reference.view_component_connector_drymate</t>
   </si>
   <si>
@@ -1486,6 +1480,12 @@
   </si>
   <si>
     <t>farm.max_seabed_temp</t>
+  </si>
+  <si>
+    <t>filter.shipping_frequency</t>
+  </si>
+  <si>
+    <t>filter.cable_corridor_shipping_frequency</t>
   </si>
 </sst>
 </file>
@@ -2097,7 +2097,7 @@
     </row>
     <row r="2" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>6</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="3" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>6</v>
@@ -4142,7 +4142,7 @@
     </row>
     <row r="2" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>220</v>
@@ -4150,7 +4150,7 @@
     </row>
     <row r="3" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>220</v>
@@ -5717,7 +5717,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B10" t="s">
         <v>242</v>
@@ -5725,7 +5725,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B11" t="s">
         <v>250</v>
@@ -6137,8 +6137,8 @@
   </sheetPr>
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6322,7 +6322,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>263</v>
@@ -6390,7 +6390,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>263</v>
@@ -6459,7 +6459,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>263</v>
@@ -6527,7 +6527,7 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>263</v>
@@ -6583,7 +6583,7 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>313</v>
@@ -6648,7 +6648,7 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>263</v>
@@ -6716,7 +6716,7 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>263</v>
@@ -6775,10 +6775,10 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B12" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C12" t="s">
         <v>329</v>
@@ -6786,10 +6786,10 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C13" t="s">
         <v>330</v>
@@ -6877,7 +6877,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C21" t="s">
         <v>336</v>
@@ -6935,7 +6935,7 @@
         <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C23" t="s">
         <v>331</v>
@@ -6946,7 +6946,7 @@
         <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C24" t="s">
         <v>333</v>
@@ -6957,7 +6957,7 @@
         <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C25" t="s">
         <v>350</v>
@@ -6968,7 +6968,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="C26" t="s">
         <v>351</v>
@@ -7046,7 +7046,7 @@
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C32" t="s">
         <v>359</v>
@@ -7057,7 +7057,7 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>474</v>
+        <v>485</v>
       </c>
       <c r="C33" t="s">
         <v>351</v>
@@ -7105,7 +7105,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Variable database table renaming in repsonce to schema changes.
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">ROOT!$A$1:$H$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Tables!$A$1:$AF$34</definedName>
     <definedName name="A">ROOT!$A$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="487">
   <si>
     <t>Identifier</t>
   </si>
@@ -732,9 +733,6 @@
     <t>Table …</t>
   </si>
   <si>
-    <t>constant_power_factor</t>
-  </si>
-  <si>
     <t>rated_voltage</t>
   </si>
   <si>
@@ -1017,9 +1015,6 @@
     <t>footprint_corner_coords</t>
   </si>
   <si>
-    <t>variable_power_factor</t>
-  </si>
-  <si>
     <t>foundation_location</t>
   </si>
   <si>
@@ -1347,9 +1342,6 @@
     <t>Group</t>
   </si>
   <si>
-    <t>filter.device</t>
-  </si>
-  <si>
     <t>reference.view_component_collection_point</t>
   </si>
   <si>
@@ -1486,6 +1478,18 @@
   </si>
   <si>
     <t>project.selected_installation_tool</t>
+  </si>
+  <si>
+    <t>filter.device_shared</t>
+  </si>
+  <si>
+    <t>filter.device_floating</t>
+  </si>
+  <si>
+    <t>power_factor_constant</t>
+  </si>
+  <si>
+    <t>power_factor_variable</t>
   </si>
 </sst>
 </file>
@@ -2059,7 +2063,7 @@
   </sheetPr>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A51" sqref="A51"/>
     </sheetView>
@@ -2091,10 +2095,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -2111,10 +2115,10 @@
         <v>93</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
@@ -2125,10 +2129,10 @@
         <v>91</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
@@ -2142,7 +2146,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H4" s="25" t="s">
         <v>8</v>
@@ -2159,7 +2163,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H5" s="25" t="s">
         <v>8</v>
@@ -2176,7 +2180,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>8</v>
@@ -2210,7 +2214,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H8" s="25" t="s">
         <v>8</v>
@@ -2227,7 +2231,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
@@ -2247,7 +2251,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>8</v>
@@ -2264,7 +2268,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H11" s="25" t="s">
         <v>8</v>
@@ -2281,7 +2285,7 @@
         <v>33</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H12" s="25" t="s">
         <v>8</v>
@@ -2295,10 +2299,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G13" s="27" t="s">
         <v>7</v>
@@ -2315,10 +2319,10 @@
         <v>6</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G14" s="27" t="s">
         <v>7</v>
@@ -2335,10 +2339,10 @@
         <v>35</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G15" s="25" t="s">
         <v>7</v>
@@ -2355,10 +2359,10 @@
         <v>37</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="25"/>
@@ -2375,10 +2379,10 @@
         <v>6</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G17" s="25" t="s">
         <v>7</v>
@@ -2395,10 +2399,10 @@
         <v>6</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G18" s="25" t="s">
         <v>7</v>
@@ -2415,10 +2419,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="25"/>
@@ -2431,16 +2435,16 @@
     </row>
     <row r="20" spans="1:8" s="25" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G20" s="25" t="s">
         <v>41</v>
@@ -2457,10 +2461,10 @@
         <v>6</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="G21" s="25" t="s">
         <v>41</v>
@@ -2477,10 +2481,10 @@
         <v>67</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>41</v>
@@ -2497,10 +2501,10 @@
         <v>67</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>41</v>
@@ -2514,10 +2518,10 @@
         <v>69</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G24" s="25" t="s">
         <v>41</v>
@@ -2559,7 +2563,7 @@
         <v>80</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
@@ -2578,10 +2582,10 @@
         <v>72</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E27" s="25"/>
       <c r="F27" s="25"/>
@@ -2600,10 +2604,10 @@
         <v>6</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E28" s="25"/>
       <c r="F28" s="25"/>
@@ -2625,7 +2629,7 @@
         <v>75</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E29" s="25"/>
       <c r="F29" s="25"/>
@@ -2638,16 +2642,16 @@
     </row>
     <row r="30" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="32" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E30" s="25"/>
       <c r="F30" s="25"/>
@@ -2660,16 +2664,16 @@
     </row>
     <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B31" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E31" s="25"/>
       <c r="F31" s="25"/>
@@ -2688,10 +2692,10 @@
         <v>6</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E32" s="25"/>
       <c r="F32" s="25"/>
@@ -2710,7 +2714,7 @@
         <v>37</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>53</v>
@@ -2735,7 +2739,7 @@
         <v>77</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E34" s="25"/>
       <c r="F34" s="25"/>
@@ -2746,16 +2750,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B35" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
@@ -2766,7 +2770,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>11</v>
@@ -2775,7 +2779,7 @@
         <v>43</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -2786,13 +2790,13 @@
     </row>
     <row r="37" spans="1:8" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="34" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>44</v>
@@ -2806,16 +2810,16 @@
     </row>
     <row r="38" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -2826,7 +2830,7 @@
     </row>
     <row r="39" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>11</v>
@@ -2835,7 +2839,7 @@
         <v>46</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -2846,7 +2850,7 @@
     </row>
     <row r="40" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>11</v>
@@ -2855,7 +2859,7 @@
         <v>47</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -2866,7 +2870,7 @@
     </row>
     <row r="41" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>11</v>
@@ -2875,7 +2879,7 @@
         <v>48</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -2886,16 +2890,16 @@
     </row>
     <row r="42" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -2906,7 +2910,7 @@
     </row>
     <row r="43" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>60</v>
@@ -2915,7 +2919,7 @@
         <v>61</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>45</v>
@@ -2923,7 +2927,7 @@
     </row>
     <row r="44" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>60</v>
@@ -2932,7 +2936,7 @@
         <v>62</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -2943,7 +2947,7 @@
     </row>
     <row r="45" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>58</v>
@@ -2952,7 +2956,7 @@
         <v>59</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -2963,16 +2967,16 @@
     </row>
     <row r="46" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="34" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B46" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
@@ -2981,16 +2985,16 @@
     </row>
     <row r="47" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
@@ -3001,16 +3005,16 @@
     </row>
     <row r="48" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
@@ -3021,16 +3025,16 @@
     </row>
     <row r="49" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -3041,7 +3045,7 @@
     </row>
     <row r="50" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>11</v>
@@ -3061,16 +3065,16 @@
     </row>
     <row r="51" spans="1:8" s="25" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
@@ -3081,7 +3085,7 @@
     </row>
     <row r="52" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>11</v>
@@ -3090,7 +3094,7 @@
         <v>56</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
@@ -3101,7 +3105,7 @@
     </row>
     <row r="53" spans="1:8" s="25" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>11</v>
@@ -3110,7 +3114,7 @@
         <v>57</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -3121,16 +3125,16 @@
     </row>
     <row r="54" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="34" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B54" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E54" s="28"/>
       <c r="F54" s="28"/>
@@ -3141,7 +3145,7 @@
     </row>
     <row r="55" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>84</v>
@@ -3161,7 +3165,7 @@
     </row>
     <row r="56" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>87</v>
@@ -3178,7 +3182,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>81</v>
@@ -3198,7 +3202,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>60</v>
@@ -3207,7 +3211,7 @@
         <v>15</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -3218,16 +3222,16 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -3240,16 +3244,16 @@
     </row>
     <row r="60" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
@@ -3260,16 +3264,16 @@
     </row>
     <row r="61" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
@@ -3280,16 +3284,16 @@
     </row>
     <row r="62" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B62" s="10" t="s">
         <v>81</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E62" s="9"/>
       <c r="F62" s="9"/>
@@ -3300,7 +3304,7 @@
     </row>
     <row r="63" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>11</v>
@@ -3309,7 +3313,7 @@
         <v>54</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -3320,7 +3324,7 @@
     </row>
     <row r="64" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>11</v>
@@ -3329,7 +3333,7 @@
         <v>55</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -3954,7 +3958,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B12" t="s">
         <v>99</v>
@@ -3975,7 +3979,7 @@
         <v>110</v>
       </c>
       <c r="H12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I12" t="s">
         <v>161</v>
@@ -3983,7 +3987,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B13" t="s">
         <v>99</v>
@@ -4006,7 +4010,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B14" t="s">
         <v>99</v>
@@ -4023,7 +4027,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B15" t="s">
         <v>165</v>
@@ -4048,7 +4052,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B17" t="s">
         <v>166</v>
@@ -4098,7 +4102,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B18" t="s">
         <v>99</v>
@@ -4243,7 +4247,7 @@
     </row>
     <row r="2" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>193</v>
@@ -4251,7 +4255,7 @@
     </row>
     <row r="3" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>193</v>
@@ -4500,7 +4504,7 @@
     </row>
     <row r="9" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>193</v>
@@ -4744,7 +4748,7 @@
     </row>
     <row r="14" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>193</v>
@@ -4817,7 +4821,7 @@
     </row>
     <row r="16" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>193</v>
@@ -4833,7 +4837,7 @@
     </row>
     <row r="18" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>199</v>
@@ -4841,7 +4845,7 @@
     </row>
     <row r="19" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>199</v>
@@ -4849,7 +4853,7 @@
     </row>
     <row r="20" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>195</v>
@@ -4857,7 +4861,7 @@
     </row>
     <row r="21" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>194</v>
@@ -4865,7 +4869,7 @@
     </row>
     <row r="22" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>194</v>
@@ -4873,7 +4877,7 @@
     </row>
     <row r="23" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>193</v>
@@ -4884,7 +4888,7 @@
     </row>
     <row r="24" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="19" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>193</v>
@@ -4892,7 +4896,7 @@
     </row>
     <row r="25" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>193</v>
@@ -4900,7 +4904,7 @@
     </row>
     <row r="26" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>193</v>
@@ -4908,7 +4912,7 @@
     </row>
     <row r="27" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="19" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>193</v>
@@ -4916,7 +4920,7 @@
     </row>
     <row r="28" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="19" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>193</v>
@@ -4933,7 +4937,7 @@
     </row>
     <row r="29" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="19" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>200</v>
@@ -5014,7 +5018,7 @@
     </row>
     <row r="32" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="19" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>194</v>
@@ -5064,7 +5068,7 @@
     </row>
     <row r="33" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>194</v>
@@ -5087,7 +5091,7 @@
     </row>
     <row r="34" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>193</v>
@@ -5157,7 +5161,7 @@
     </row>
     <row r="42" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="19" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B42" s="19" t="s">
         <v>193</v>
@@ -5165,7 +5169,7 @@
     </row>
     <row r="43" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="19" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B43" s="19" t="s">
         <v>195</v>
@@ -5211,7 +5215,7 @@
     </row>
     <row r="48" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="19" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B48" s="19" t="s">
         <v>193</v>
@@ -5219,7 +5223,7 @@
     </row>
     <row r="49" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="19" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B49" s="19" t="s">
         <v>194</v>
@@ -5227,7 +5231,7 @@
     </row>
     <row r="50" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="19" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B50" s="19" t="s">
         <v>194</v>
@@ -5235,7 +5239,7 @@
     </row>
     <row r="51" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="19" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B51" s="19" t="s">
         <v>194</v>
@@ -5243,7 +5247,7 @@
     </row>
     <row r="52" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="19" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>193</v>
@@ -5818,7 +5822,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B10" t="s">
         <v>215</v>
@@ -5826,7 +5830,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B11" t="s">
         <v>223</v>
@@ -5921,7 +5925,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B21" t="s">
         <v>196</v>
@@ -5929,7 +5933,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B22" t="s">
         <v>226</v>
@@ -5937,7 +5941,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B23" t="s">
         <v>226</v>
@@ -5945,7 +5949,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B24" t="s">
         <v>226</v>
@@ -5956,7 +5960,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B25" t="s">
         <v>205</v>
@@ -5964,7 +5968,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B26" t="s">
         <v>210</v>
@@ -5980,7 +5984,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B28" t="s">
         <v>217</v>
@@ -5988,7 +5992,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B29" t="s">
         <v>219</v>
@@ -5996,7 +6000,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B30" t="s">
         <v>196</v>
@@ -6046,7 +6050,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B31" t="s">
         <v>196</v>
@@ -6124,7 +6128,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B38" t="s">
         <v>210</v>
@@ -6138,7 +6142,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B39" t="s">
         <v>210</v>
@@ -6152,7 +6156,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B40" t="s">
         <v>196</v>
@@ -6211,7 +6215,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B44" t="s">
         <v>196</v>
@@ -6219,7 +6223,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B45" t="s">
         <v>196</v>
@@ -6238,8 +6242,8 @@
   </sheetPr>
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6299,901 +6303,968 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C2" t="s">
-        <v>234</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C3" t="s">
-        <v>235</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>440</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="I4" t="s">
-        <v>242</v>
-      </c>
-      <c r="J4" t="s">
-        <v>243</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="M4" t="s">
-        <v>246</v>
-      </c>
-      <c r="N4" t="s">
-        <v>247</v>
-      </c>
-      <c r="O4" t="s">
-        <v>248</v>
-      </c>
-      <c r="P4" t="s">
-        <v>249</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>250</v>
-      </c>
-      <c r="R4" t="s">
-        <v>251</v>
-      </c>
-      <c r="S4" t="s">
-        <v>252</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="U4" t="s">
-        <v>254</v>
-      </c>
-      <c r="V4" t="s">
-        <v>255</v>
-      </c>
-      <c r="W4" t="s">
-        <v>256</v>
-      </c>
-      <c r="X4" t="s">
-        <v>257</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>258</v>
-      </c>
-      <c r="Z4" s="16" t="s">
-        <v>259</v>
-      </c>
-      <c r="AA4" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="AB4" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="AC4" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="AD4" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>265</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
       <c r="AG4" s="1"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>443</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="I5" t="s">
-        <v>247</v>
-      </c>
-      <c r="J5" t="s">
-        <v>248</v>
-      </c>
-      <c r="K5" t="s">
-        <v>269</v>
-      </c>
-      <c r="L5" t="s">
-        <v>270</v>
-      </c>
-      <c r="M5" t="s">
-        <v>249</v>
-      </c>
-      <c r="N5" t="s">
-        <v>250</v>
-      </c>
-      <c r="O5" t="s">
-        <v>255</v>
-      </c>
-      <c r="P5" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>271</v>
-      </c>
-      <c r="R5" t="s">
-        <v>272</v>
-      </c>
-      <c r="S5" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="T5" s="16" t="s">
-        <v>274</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>265</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>444</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="I6" t="s">
-        <v>279</v>
-      </c>
-      <c r="J6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K6" t="s">
-        <v>281</v>
-      </c>
-      <c r="L6" t="s">
-        <v>282</v>
-      </c>
-      <c r="M6" t="s">
-        <v>249</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="P6" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>284</v>
-      </c>
-      <c r="R6" t="s">
-        <v>285</v>
-      </c>
-      <c r="S6" t="s">
-        <v>255</v>
-      </c>
-      <c r="T6" t="s">
-        <v>272</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="W6" s="1"/>
+        <v>438</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
-        <v>26</v>
+      <c r="A7" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>445</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="I7" t="s">
-        <v>279</v>
-      </c>
-      <c r="J7" t="s">
-        <v>280</v>
-      </c>
-      <c r="K7" t="s">
-        <v>281</v>
-      </c>
-      <c r="L7" t="s">
-        <v>282</v>
-      </c>
-      <c r="M7" t="s">
-        <v>249</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="P7" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>284</v>
-      </c>
-      <c r="R7" t="s">
-        <v>285</v>
-      </c>
-      <c r="S7" t="s">
-        <v>255</v>
-      </c>
-      <c r="T7" t="s">
-        <v>272</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>265</v>
-      </c>
+        <v>439</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
-        <v>28</v>
+      <c r="A8" s="19" t="s">
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>446</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="I8" t="s">
-        <v>248</v>
-      </c>
-      <c r="J8" t="s">
-        <v>254</v>
-      </c>
-      <c r="K8" t="s">
-        <v>256</v>
-      </c>
-      <c r="L8" t="s">
-        <v>250</v>
-      </c>
-      <c r="M8" t="s">
-        <v>249</v>
-      </c>
-      <c r="N8" t="s">
-        <v>271</v>
-      </c>
-      <c r="O8" t="s">
-        <v>272</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
+        <v>452</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>447</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="J9" t="s">
-        <v>292</v>
-      </c>
-      <c r="K9" t="s">
-        <v>293</v>
-      </c>
-      <c r="L9" t="s">
-        <v>294</v>
-      </c>
-      <c r="M9" t="s">
-        <v>249</v>
-      </c>
-      <c r="N9" t="s">
-        <v>250</v>
-      </c>
-      <c r="O9" t="s">
-        <v>253</v>
-      </c>
-      <c r="P9" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>271</v>
-      </c>
-      <c r="R9" t="s">
-        <v>272</v>
-      </c>
-      <c r="S9" s="16" t="s">
-        <v>295</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>265</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>485</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>448</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="I10" t="s">
-        <v>247</v>
-      </c>
-      <c r="J10" t="s">
-        <v>248</v>
-      </c>
-      <c r="K10" t="s">
-        <v>269</v>
-      </c>
-      <c r="L10" t="s">
-        <v>270</v>
-      </c>
-      <c r="M10" t="s">
-        <v>249</v>
-      </c>
-      <c r="N10" t="s">
-        <v>250</v>
-      </c>
-      <c r="O10" t="s">
-        <v>255</v>
-      </c>
-      <c r="P10" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>271</v>
-      </c>
-      <c r="R10" t="s">
-        <v>272</v>
-      </c>
-      <c r="S10" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="T10" s="16" t="s">
-        <v>274</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>265</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>449</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D11" t="s">
-        <v>235</v>
-      </c>
-      <c r="E11" t="s">
-        <v>296</v>
-      </c>
-      <c r="F11" t="s">
-        <v>297</v>
-      </c>
-      <c r="G11" t="s">
-        <v>298</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="I11" t="s">
-        <v>256</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="L11" t="s">
-        <v>301</v>
-      </c>
-      <c r="M11" t="s">
-        <v>253</v>
-      </c>
-      <c r="N11" t="s">
-        <v>250</v>
-      </c>
-      <c r="O11" t="s">
-        <v>249</v>
-      </c>
-      <c r="P11" t="s">
-        <v>271</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>272</v>
-      </c>
-      <c r="R11" t="s">
-        <v>254</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>265</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="H11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>452</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>451</v>
+        <v>484</v>
       </c>
       <c r="C12" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>484</v>
+      </c>
+      <c r="C13" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
+        <v>483</v>
+      </c>
+      <c r="C14" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A15" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>483</v>
+      </c>
+      <c r="C15" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A16" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>483</v>
+      </c>
+      <c r="C16" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="B17" t="s">
+        <v>483</v>
+      </c>
+      <c r="C17" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A18" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="B18" t="s">
+        <v>448</v>
+      </c>
+      <c r="C18" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A19" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="B19" t="s">
+        <v>448</v>
+      </c>
+      <c r="C19" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
-        <v>453</v>
-      </c>
-      <c r="B13" t="s">
-        <v>451</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A20" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>448</v>
+      </c>
+      <c r="C20" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>441</v>
-      </c>
-      <c r="C14" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>441</v>
-      </c>
-      <c r="C15" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" t="s">
-        <v>441</v>
-      </c>
-      <c r="C16" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>441</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>448</v>
+      </c>
+      <c r="C21" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>441</v>
-      </c>
-      <c r="C18" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" t="s">
-        <v>439</v>
-      </c>
-      <c r="C19" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" t="s">
-        <v>439</v>
-      </c>
-      <c r="C20" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>450</v>
-      </c>
-      <c r="C21" t="s">
-        <v>309</v>
-      </c>
-      <c r="D21" t="s">
-        <v>310</v>
-      </c>
-      <c r="E21" t="s">
-        <v>311</v>
-      </c>
-      <c r="F21" t="s">
-        <v>312</v>
-      </c>
-      <c r="G21" t="s">
-        <v>313</v>
-      </c>
-      <c r="H21" t="s">
-        <v>314</v>
-      </c>
-      <c r="I21" t="s">
-        <v>315</v>
-      </c>
-      <c r="J21" t="s">
-        <v>316</v>
-      </c>
-      <c r="K21" t="s">
-        <v>317</v>
-      </c>
-      <c r="L21" t="s">
-        <v>318</v>
-      </c>
-      <c r="M21" t="s">
-        <v>319</v>
-      </c>
-      <c r="N21" t="s">
-        <v>320</v>
-      </c>
-      <c r="O21" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="C22" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
         <v>451</v>
       </c>
       <c r="C23" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+      <c r="D23" t="s">
+        <v>324</v>
+      </c>
+      <c r="E23" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C24" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>73</v>
+        <v>308</v>
+      </c>
+      <c r="D24" t="s">
+        <v>309</v>
+      </c>
+      <c r="E24" t="s">
+        <v>310</v>
+      </c>
+      <c r="F24" t="s">
+        <v>311</v>
+      </c>
+      <c r="G24" t="s">
+        <v>312</v>
+      </c>
+      <c r="H24" t="s">
+        <v>313</v>
+      </c>
+      <c r="I24" t="s">
+        <v>314</v>
+      </c>
+      <c r="J24" t="s">
+        <v>315</v>
+      </c>
+      <c r="K24" t="s">
+        <v>316</v>
+      </c>
+      <c r="L24" t="s">
+        <v>317</v>
+      </c>
+      <c r="M24" t="s">
+        <v>318</v>
+      </c>
+      <c r="N24" t="s">
+        <v>319</v>
+      </c>
+      <c r="O24" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A25" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>451</v>
-      </c>
-      <c r="C25" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>52</v>
+        <v>441</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="I25" t="s">
+        <v>278</v>
+      </c>
+      <c r="J25" t="s">
+        <v>279</v>
+      </c>
+      <c r="K25" t="s">
+        <v>280</v>
+      </c>
+      <c r="L25" t="s">
+        <v>281</v>
+      </c>
+      <c r="M25" t="s">
+        <v>248</v>
+      </c>
+      <c r="N25" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="O25" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="P25" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>283</v>
+      </c>
+      <c r="R25" t="s">
+        <v>284</v>
+      </c>
+      <c r="S25" t="s">
+        <v>254</v>
+      </c>
+      <c r="T25" t="s">
+        <v>271</v>
+      </c>
+      <c r="U25" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="V25" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="W25" s="16"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A26" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>454</v>
-      </c>
-      <c r="C26" t="s">
-        <v>324</v>
-      </c>
-      <c r="D26" t="s">
-        <v>325</v>
-      </c>
-      <c r="E26" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
-        <v>78</v>
+        <v>442</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="I26" t="s">
+        <v>278</v>
+      </c>
+      <c r="J26" t="s">
+        <v>279</v>
+      </c>
+      <c r="K26" t="s">
+        <v>280</v>
+      </c>
+      <c r="L26" t="s">
+        <v>281</v>
+      </c>
+      <c r="M26" t="s">
+        <v>248</v>
+      </c>
+      <c r="N26" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="O26" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="P26" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>283</v>
+      </c>
+      <c r="R26" t="s">
+        <v>284</v>
+      </c>
+      <c r="S26" t="s">
+        <v>254</v>
+      </c>
+      <c r="T26" t="s">
+        <v>271</v>
+      </c>
+      <c r="U26" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="V26" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A27" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>439</v>
-      </c>
-      <c r="C27" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+        <v>437</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="I27" t="s">
+        <v>241</v>
+      </c>
+      <c r="J27" t="s">
+        <v>242</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="M27" t="s">
+        <v>245</v>
+      </c>
+      <c r="N27" t="s">
+        <v>246</v>
+      </c>
+      <c r="O27" t="s">
+        <v>247</v>
+      </c>
+      <c r="P27" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>249</v>
+      </c>
+      <c r="R27" t="s">
+        <v>250</v>
+      </c>
+      <c r="S27" t="s">
+        <v>251</v>
+      </c>
+      <c r="T27" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="U27" t="s">
+        <v>253</v>
+      </c>
+      <c r="V27" t="s">
+        <v>254</v>
+      </c>
+      <c r="W27" t="s">
+        <v>255</v>
+      </c>
+      <c r="X27" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z27" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="AA27" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="AB27" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="AC27" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="AD27" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE27" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="AF27" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>439</v>
-      </c>
-      <c r="C28" t="s">
+        <v>437</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>439</v>
-      </c>
-      <c r="C29" t="s">
+        <v>437</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>90</v>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A30" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="B30" t="s">
         <v>440</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>92</v>
+        <v>265</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="I30" t="s">
+        <v>246</v>
+      </c>
+      <c r="J30" t="s">
+        <v>247</v>
+      </c>
+      <c r="K30" t="s">
+        <v>268</v>
+      </c>
+      <c r="L30" t="s">
+        <v>269</v>
+      </c>
+      <c r="M30" t="s">
+        <v>248</v>
+      </c>
+      <c r="N30" t="s">
+        <v>249</v>
+      </c>
+      <c r="O30" t="s">
+        <v>254</v>
+      </c>
+      <c r="P30" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>270</v>
+      </c>
+      <c r="R30" t="s">
+        <v>271</v>
+      </c>
+      <c r="S30" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="T30" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="U30" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="V30" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A31" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>34</v>
+        <v>265</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="I31" t="s">
+        <v>246</v>
+      </c>
+      <c r="J31" t="s">
+        <v>247</v>
+      </c>
+      <c r="K31" t="s">
+        <v>268</v>
+      </c>
+      <c r="L31" t="s">
+        <v>269</v>
+      </c>
+      <c r="M31" t="s">
+        <v>248</v>
+      </c>
+      <c r="N31" t="s">
+        <v>249</v>
+      </c>
+      <c r="O31" t="s">
+        <v>254</v>
+      </c>
+      <c r="P31" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>270</v>
+      </c>
+      <c r="R31" t="s">
+        <v>271</v>
+      </c>
+      <c r="S31" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="T31" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="U31" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="V31" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A32" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>442</v>
-      </c>
-      <c r="C32" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>36</v>
+        <v>446</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D32" t="s">
+        <v>234</v>
+      </c>
+      <c r="E32" t="s">
+        <v>295</v>
+      </c>
+      <c r="F32" t="s">
+        <v>296</v>
+      </c>
+      <c r="G32" t="s">
+        <v>297</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="I32" t="s">
+        <v>255</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="K32" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="L32" t="s">
+        <v>300</v>
+      </c>
+      <c r="M32" t="s">
+        <v>252</v>
+      </c>
+      <c r="N32" t="s">
+        <v>249</v>
+      </c>
+      <c r="O32" t="s">
+        <v>248</v>
+      </c>
+      <c r="P32" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>271</v>
+      </c>
+      <c r="R32" t="s">
+        <v>253</v>
+      </c>
+      <c r="S32" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="T32" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A33" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>455</v>
-      </c>
-      <c r="C33" t="s">
-        <v>324</v>
-      </c>
-      <c r="D33" t="s">
-        <v>325</v>
-      </c>
-      <c r="E33" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+        <v>443</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="I33" t="s">
+        <v>247</v>
+      </c>
+      <c r="J33" t="s">
+        <v>253</v>
+      </c>
+      <c r="K33" t="s">
+        <v>255</v>
+      </c>
+      <c r="L33" t="s">
+        <v>249</v>
+      </c>
+      <c r="M33" t="s">
+        <v>248</v>
+      </c>
+      <c r="N33" t="s">
+        <v>270</v>
+      </c>
+      <c r="O33" t="s">
+        <v>271</v>
+      </c>
+      <c r="P33" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q33" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
-        <v>424</v>
+        <v>30</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>439</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>427</v>
-      </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
+        <v>444</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="J34" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="M34" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="O34" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="P34" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>270</v>
+      </c>
+      <c r="R34" t="s">
+        <v>271</v>
+      </c>
+      <c r="S34" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="T34" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="U34" s="16" t="s">
+        <v>264</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AF34">
+    <sortState ref="A2:AF34">
+      <sortCondition ref="B1:B34"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -7223,27 +7294,27 @@
         <v>188</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>334</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>335</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -7251,46 +7322,46 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D3" t="s">
         <v>339</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>340</v>
-      </c>
-      <c r="D3" t="s">
-        <v>341</v>
-      </c>
-      <c r="E3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>339</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="E5" s="19" t="s">
         <v>340</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>341</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data model updates and database connections
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="491">
   <si>
     <t>Identifier</t>
   </si>
@@ -1168,9 +1168,6 @@
     <t>Defines the number of control signal pairs per device.</t>
   </si>
   <si>
-    <t>The type of control signal used in the array, accepts 'fibre optic'.</t>
-  </si>
-  <si>
     <t>Maximum Number of Devices per Radial String</t>
   </si>
   <si>
@@ -1405,15 +1402,6 @@
     <t>project.array_efficiency</t>
   </si>
   <si>
-    <t>project.control_signal_cable</t>
-  </si>
-  <si>
-    <t>project.control_signal_channels</t>
-  </si>
-  <si>
-    <t>project.control_signal_type</t>
-  </si>
-  <si>
     <t>project.devices_per_string</t>
   </si>
   <si>
@@ -1490,19 +1478,50 @@
   </si>
   <si>
     <t>power_factor_variable</t>
+  </si>
+  <si>
+    <t>device.control_signal_cable</t>
+  </si>
+  <si>
+    <t>device.control_signal_channels</t>
+  </si>
+  <si>
+    <t>device.control_signal_type</t>
+  </si>
+  <si>
+    <t>control_signal_cable</t>
+  </si>
+  <si>
+    <t>control_signal_channels</t>
+  </si>
+  <si>
+    <t>control_signal_type</t>
+  </si>
+  <si>
+    <t>Fibre Optic</t>
+  </si>
+  <si>
+    <t>The type of control signal used in the device. Currently only accepts 'Fibre Optic'.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1621,27 +1640,27 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1649,13 +1668,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1667,22 +1686,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -2063,9 +2086,9 @@
   </sheetPr>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A51" sqref="A51"/>
+      <selection pane="topRight" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2095,10 +2118,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -2115,10 +2138,10 @@
         <v>93</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
@@ -2129,10 +2152,10 @@
         <v>91</v>
       </c>
       <c r="C3" s="25" t="s">
+        <v>412</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>413</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
@@ -2435,16 +2458,16 @@
     </row>
     <row r="20" spans="1:8" s="25" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="D20" s="26" t="s">
         <v>423</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>424</v>
       </c>
       <c r="G20" s="25" t="s">
         <v>41</v>
@@ -2461,10 +2484,10 @@
         <v>6</v>
       </c>
       <c r="C21" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="D21" s="26" t="s">
         <v>401</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>402</v>
       </c>
       <c r="G21" s="25" t="s">
         <v>41</v>
@@ -2481,10 +2504,10 @@
         <v>67</v>
       </c>
       <c r="C22" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="D22" s="26" t="s">
         <v>397</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>398</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>41</v>
@@ -2501,10 +2524,10 @@
         <v>67</v>
       </c>
       <c r="C23" s="25" t="s">
+        <v>418</v>
+      </c>
+      <c r="D23" s="26" t="s">
         <v>419</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>420</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>41</v>
@@ -2518,10 +2541,10 @@
         <v>69</v>
       </c>
       <c r="C24" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="D24" s="26" t="s">
         <v>399</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>400</v>
       </c>
       <c r="G24" s="25" t="s">
         <v>41</v>
@@ -2563,7 +2586,7 @@
         <v>80</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
@@ -2582,10 +2605,10 @@
         <v>72</v>
       </c>
       <c r="C27" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="D27" s="26" t="s">
         <v>405</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>406</v>
       </c>
       <c r="E27" s="25"/>
       <c r="F27" s="25"/>
@@ -2629,7 +2652,7 @@
         <v>75</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E29" s="25"/>
       <c r="F29" s="25"/>
@@ -2642,7 +2665,7 @@
     </row>
     <row r="30" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="32" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>6</v>
@@ -2664,7 +2687,7 @@
     </row>
     <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="32" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B31" s="25" t="s">
         <v>6</v>
@@ -2692,10 +2715,10 @@
         <v>6</v>
       </c>
       <c r="C32" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="D32" s="26" t="s">
         <v>409</v>
-      </c>
-      <c r="D32" s="26" t="s">
-        <v>410</v>
       </c>
       <c r="E32" s="25"/>
       <c r="F32" s="25"/>
@@ -2714,7 +2737,7 @@
         <v>37</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>53</v>
@@ -2739,7 +2762,7 @@
         <v>77</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E34" s="25"/>
       <c r="F34" s="25"/>
@@ -2750,16 +2773,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B35" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="28" t="s">
+        <v>428</v>
+      </c>
+      <c r="D35" s="29" t="s">
         <v>429</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>430</v>
       </c>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
@@ -2770,7 +2793,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>11</v>
@@ -2790,7 +2813,7 @@
     </row>
     <row r="37" spans="1:8" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="34" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>11</v>
@@ -2810,16 +2833,16 @@
     </row>
     <row r="38" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C38" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="D38" s="21" t="s">
         <v>394</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>395</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -2828,78 +2851,69 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="4" t="s">
+    <row r="39" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="25" t="s">
+        <v>483</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="26" t="s">
         <v>377</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4" t="s">
+      <c r="H39" s="25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="4" t="s">
+    <row r="40" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="25" t="s">
+        <v>484</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="26" t="s">
         <v>378</v>
       </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4" t="s">
+      <c r="H40" s="25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
-        <v>460</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="4" t="s">
+    <row r="41" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="36" t="s">
+        <v>485</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4" t="s">
+      <c r="D41" s="35" t="s">
+        <v>490</v>
+      </c>
+      <c r="H41" s="25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>380</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>381</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -2910,7 +2924,7 @@
     </row>
     <row r="43" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>60</v>
@@ -2919,7 +2933,7 @@
         <v>61</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>45</v>
@@ -2927,7 +2941,7 @@
     </row>
     <row r="44" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>60</v>
@@ -2936,7 +2950,7 @@
         <v>62</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -2947,7 +2961,7 @@
     </row>
     <row r="45" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>58</v>
@@ -2956,7 +2970,7 @@
         <v>59</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -2967,16 +2981,16 @@
     </row>
     <row r="46" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="34" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B46" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C46" s="28" t="s">
+        <v>432</v>
+      </c>
+      <c r="D46" s="29" t="s">
         <v>433</v>
-      </c>
-      <c r="D46" s="29" t="s">
-        <v>434</v>
       </c>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
@@ -2985,7 +2999,7 @@
     </row>
     <row r="47" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>11</v>
@@ -3005,7 +3019,7 @@
     </row>
     <row r="48" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>11</v>
@@ -3025,7 +3039,7 @@
     </row>
     <row r="49" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>11</v>
@@ -3045,7 +3059,7 @@
     </row>
     <row r="50" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>11</v>
@@ -3065,16 +3079,16 @@
     </row>
     <row r="51" spans="1:8" s="25" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>382</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>383</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
@@ -3085,7 +3099,7 @@
     </row>
     <row r="52" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>11</v>
@@ -3094,7 +3108,7 @@
         <v>56</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
@@ -3105,7 +3119,7 @@
     </row>
     <row r="53" spans="1:8" s="25" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>11</v>
@@ -3114,7 +3128,7 @@
         <v>57</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -3125,16 +3139,16 @@
     </row>
     <row r="54" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="34" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B54" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C54" s="28" t="s">
+        <v>430</v>
+      </c>
+      <c r="D54" s="29" t="s">
         <v>431</v>
-      </c>
-      <c r="D54" s="29" t="s">
-        <v>432</v>
       </c>
       <c r="E54" s="28"/>
       <c r="F54" s="28"/>
@@ -3145,7 +3159,7 @@
     </row>
     <row r="55" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>84</v>
@@ -3165,7 +3179,7 @@
     </row>
     <row r="56" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>87</v>
@@ -3182,7 +3196,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>81</v>
@@ -3202,7 +3216,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>60</v>
@@ -3211,7 +3225,7 @@
         <v>15</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -3222,16 +3236,16 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C59" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>385</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>386</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -3244,16 +3258,16 @@
     </row>
     <row r="60" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C60" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="D60" s="21" t="s">
         <v>403</v>
-      </c>
-      <c r="D60" s="21" t="s">
-        <v>404</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
@@ -3264,16 +3278,16 @@
     </row>
     <row r="61" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C61" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="D61" s="22" t="s">
         <v>407</v>
-      </c>
-      <c r="D61" s="22" t="s">
-        <v>408</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
@@ -3284,16 +3298,16 @@
     </row>
     <row r="62" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B62" s="10" t="s">
         <v>81</v>
       </c>
       <c r="C62" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="D62" s="23" t="s">
         <v>417</v>
-      </c>
-      <c r="D62" s="23" t="s">
-        <v>418</v>
       </c>
       <c r="E62" s="9"/>
       <c r="F62" s="9"/>
@@ -3304,7 +3318,7 @@
     </row>
     <row r="63" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>11</v>
@@ -3313,7 +3327,7 @@
         <v>54</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -3324,7 +3338,7 @@
     </row>
     <row r="64" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>11</v>
@@ -3333,7 +3347,7 @@
         <v>55</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -3958,7 +3972,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B12" t="s">
         <v>99</v>
@@ -3979,7 +3993,7 @@
         <v>110</v>
       </c>
       <c r="H12" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I12" t="s">
         <v>161</v>
@@ -3987,7 +4001,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B13" t="s">
         <v>99</v>
@@ -4010,7 +4024,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B14" t="s">
         <v>99</v>
@@ -4027,7 +4041,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B15" t="s">
         <v>165</v>
@@ -4052,7 +4066,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B17" t="s">
         <v>166</v>
@@ -4102,7 +4116,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B18" t="s">
         <v>99</v>
@@ -4247,7 +4261,7 @@
     </row>
     <row r="2" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>193</v>
@@ -4255,7 +4269,7 @@
     </row>
     <row r="3" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>193</v>
@@ -4504,7 +4518,7 @@
     </row>
     <row r="9" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>193</v>
@@ -4748,7 +4762,7 @@
     </row>
     <row r="14" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>193</v>
@@ -4821,7 +4835,7 @@
     </row>
     <row r="16" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>193</v>
@@ -4837,7 +4851,7 @@
     </row>
     <row r="18" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>199</v>
@@ -4845,7 +4859,7 @@
     </row>
     <row r="19" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
-        <v>458</v>
+        <v>483</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>199</v>
@@ -4853,7 +4867,7 @@
     </row>
     <row r="20" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
-        <v>459</v>
+        <v>484</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>195</v>
@@ -4861,7 +4875,7 @@
     </row>
     <row r="21" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
-        <v>460</v>
+        <v>485</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>194</v>
@@ -4869,7 +4883,7 @@
     </row>
     <row r="22" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>194</v>
@@ -4877,7 +4891,7 @@
     </row>
     <row r="23" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>193</v>
@@ -4888,7 +4902,7 @@
     </row>
     <row r="24" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="19" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>193</v>
@@ -4896,7 +4910,7 @@
     </row>
     <row r="25" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>193</v>
@@ -4904,7 +4918,7 @@
     </row>
     <row r="26" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>193</v>
@@ -4912,7 +4926,7 @@
     </row>
     <row r="27" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="19" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>193</v>
@@ -4920,7 +4934,7 @@
     </row>
     <row r="28" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="19" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>193</v>
@@ -4937,7 +4951,7 @@
     </row>
     <row r="29" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="19" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>200</v>
@@ -5018,7 +5032,7 @@
     </row>
     <row r="32" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="19" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>194</v>
@@ -5068,7 +5082,7 @@
     </row>
     <row r="33" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>194</v>
@@ -5091,7 +5105,7 @@
     </row>
     <row r="34" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>193</v>
@@ -5161,7 +5175,7 @@
     </row>
     <row r="42" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="19" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B42" s="19" t="s">
         <v>193</v>
@@ -5169,7 +5183,7 @@
     </row>
     <row r="43" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="19" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B43" s="19" t="s">
         <v>195</v>
@@ -5215,7 +5229,7 @@
     </row>
     <row r="48" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="19" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B48" s="19" t="s">
         <v>193</v>
@@ -5223,7 +5237,7 @@
     </row>
     <row r="49" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="19" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B49" s="19" t="s">
         <v>194</v>
@@ -5231,7 +5245,7 @@
     </row>
     <row r="50" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="19" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B50" s="19" t="s">
         <v>194</v>
@@ -5239,7 +5253,7 @@
     </row>
     <row r="51" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="19" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B51" s="19" t="s">
         <v>194</v>
@@ -5247,7 +5261,7 @@
     </row>
     <row r="52" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="19" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>193</v>
@@ -5822,7 +5836,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B10" t="s">
         <v>215</v>
@@ -5830,7 +5844,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B11" t="s">
         <v>223</v>
@@ -5925,7 +5939,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>460</v>
+        <v>485</v>
       </c>
       <c r="B21" t="s">
         <v>196</v>
@@ -5933,7 +5947,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B22" t="s">
         <v>226</v>
@@ -5941,7 +5955,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B23" t="s">
         <v>226</v>
@@ -5949,7 +5963,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B24" t="s">
         <v>226</v>
@@ -5960,7 +5974,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B25" t="s">
         <v>205</v>
@@ -5968,7 +5982,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B26" t="s">
         <v>210</v>
@@ -5984,7 +5998,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B28" t="s">
         <v>217</v>
@@ -5992,7 +6006,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B29" t="s">
         <v>219</v>
@@ -6000,7 +6014,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B30" t="s">
         <v>196</v>
@@ -6050,7 +6064,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B31" t="s">
         <v>196</v>
@@ -6128,7 +6142,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B38" t="s">
         <v>210</v>
@@ -6142,7 +6156,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B39" t="s">
         <v>210</v>
@@ -6156,7 +6170,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B40" t="s">
         <v>196</v>
@@ -6215,7 +6229,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B44" t="s">
         <v>196</v>
@@ -6223,7 +6237,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B45" t="s">
         <v>196</v>
@@ -6240,10 +6254,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:AG34"/>
+  <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6306,7 +6320,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C2" t="s">
         <v>301</v>
@@ -6317,7 +6331,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C3" t="s">
         <v>302</v>
@@ -6328,7 +6342,7 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>303</v>
@@ -6355,7 +6369,7 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>304</v>
@@ -6375,7 +6389,7 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>305</v>
@@ -6396,7 +6410,7 @@
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>330</v>
@@ -6416,7 +6430,7 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>323</v>
@@ -6441,10 +6455,10 @@
         <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -6461,7 +6475,7 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>234</v>
@@ -6481,7 +6495,7 @@
         <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>306</v>
@@ -6497,7 +6511,7 @@
         <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C12" t="s">
         <v>307</v>
@@ -6508,7 +6522,7 @@
         <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C13" t="s">
         <v>321</v>
@@ -6519,7 +6533,7 @@
         <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C14" t="s">
         <v>326</v>
@@ -6530,7 +6544,7 @@
         <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C15" t="s">
         <v>327</v>
@@ -6541,29 +6555,29 @@
         <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C16" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B17" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B18" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C18" t="s">
         <v>301</v>
@@ -6571,10 +6585,10 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C19" t="s">
         <v>302</v>
@@ -6585,7 +6599,7 @@
         <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C20" t="s">
         <v>303</v>
@@ -6596,7 +6610,7 @@
         <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C21" t="s">
         <v>305</v>
@@ -6607,7 +6621,7 @@
         <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C22" t="s">
         <v>322</v>
@@ -6618,7 +6632,7 @@
         <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C23" t="s">
         <v>323</v>
@@ -6635,7 +6649,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C24" t="s">
         <v>308</v>
@@ -6682,7 +6696,7 @@
         <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>235</v>
@@ -6751,7 +6765,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>235</v>
@@ -6819,7 +6833,7 @@
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>235</v>
@@ -6917,7 +6931,7 @@
         <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>235</v>
@@ -6931,7 +6945,7 @@
         <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>235</v>
@@ -6945,7 +6959,7 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>235</v>
@@ -7013,7 +7027,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>235</v>
@@ -7081,7 +7095,7 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>235</v>
@@ -7143,7 +7157,7 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>235</v>
@@ -7199,7 +7213,7 @@
         <v>30</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>285</v>
@@ -7257,6 +7271,39 @@
       </c>
       <c r="U34" s="16" t="s">
         <v>264</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="19" t="s">
+        <v>483</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="19" t="s">
+        <v>485</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -7275,10 +7322,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7308,7 +7355,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B2" t="s">
         <v>335</v>
@@ -7336,20 +7383,20 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>425</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>426</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>427</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>337</v>
@@ -7362,6 +7409,14 @@
       </c>
       <c r="E5" s="19" t="s">
         <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
+        <v>485</v>
+      </c>
+      <c r="B6" t="s">
+        <v>489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue with chosen trenching type definition.
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="456">
   <si>
     <t>Identifier</t>
   </si>
@@ -2002,9 +2002,9 @@
   </sheetPr>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G11" sqref="G11"/>
+      <selection pane="topRight" activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4955,10 +4955,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:AE43"/>
+  <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5532,344 +5532,320 @@
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>408</v>
+      <c r="A16" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
-        <v>57</v>
+      <c r="A17" t="s">
+        <v>69</v>
       </c>
       <c r="B17" t="s">
         <v>172</v>
       </c>
+      <c r="C17" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>69</v>
+      <c r="A18" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="B18" t="s">
+        <v>185</v>
+      </c>
+      <c r="C18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
         <v>172</v>
-      </c>
-      <c r="C18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" t="s">
-        <v>185</v>
-      </c>
-      <c r="C19" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="A21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>172</v>
       </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>372</v>
       </c>
       <c r="B24" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B25" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>371</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>182</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>184</v>
-      </c>
-      <c r="E27" s="19"/>
+        <v>179</v>
+      </c>
+      <c r="C27" t="s">
+        <v>183</v>
+      </c>
+      <c r="D27" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" t="s">
-        <v>179</v>
-      </c>
-      <c r="C28" t="s">
-        <v>183</v>
-      </c>
-      <c r="D28" t="s">
-        <v>183</v>
-      </c>
+      <c r="A28" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+      <c r="A29" t="s">
+        <v>392</v>
+      </c>
+      <c r="B29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29" t="s">
+        <v>172</v>
+      </c>
+      <c r="F29" t="s">
+        <v>172</v>
+      </c>
+      <c r="G29" t="s">
+        <v>172</v>
+      </c>
+      <c r="H29" t="s">
+        <v>161</v>
+      </c>
+      <c r="I29" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="16" t="s">
-        <v>400</v>
+      <c r="A30" s="19" t="s">
+        <v>377</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
-      </c>
-      <c r="C31" t="s">
-        <v>172</v>
-      </c>
-      <c r="D31" t="s">
-        <v>161</v>
-      </c>
-      <c r="E31" t="s">
-        <v>172</v>
-      </c>
-      <c r="F31" t="s">
-        <v>172</v>
-      </c>
-      <c r="G31" t="s">
-        <v>172</v>
-      </c>
-      <c r="H31" t="s">
-        <v>161</v>
-      </c>
-      <c r="I31" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="19" t="s">
-        <v>377</v>
+      <c r="A32" t="s">
+        <v>382</v>
       </c>
       <c r="B32" t="s">
-        <v>172</v>
+        <v>185</v>
+      </c>
+      <c r="C32" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="B33" t="s">
-        <v>168</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="B34" t="s">
-        <v>185</v>
-      </c>
-      <c r="C34" t="s">
-        <v>185</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>386</v>
+      <c r="A35" s="19" t="s">
+        <v>397</v>
       </c>
       <c r="B35" t="s">
-        <v>434</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
+        <v>172</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>387</v>
+      <c r="A36" s="19" t="s">
+        <v>398</v>
       </c>
       <c r="B36" t="s">
-        <v>179</v>
-      </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
+        <v>172</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A37" s="16" t="s">
-        <v>401</v>
+      <c r="A37" t="s">
+        <v>393</v>
       </c>
       <c r="B37" t="s">
         <v>161</v>
       </c>
+      <c r="C37" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="F37" t="s">
+        <v>172</v>
+      </c>
+      <c r="G37" t="s">
+        <v>172</v>
+      </c>
+      <c r="H37" t="s">
+        <v>172</v>
+      </c>
+      <c r="I37" t="s">
+        <v>161</v>
+      </c>
+      <c r="J37" t="s">
+        <v>180</v>
+      </c>
+      <c r="K37" t="s">
+        <v>180</v>
+      </c>
+      <c r="L37" t="s">
+        <v>180</v>
+      </c>
+      <c r="M37" t="s">
+        <v>180</v>
+      </c>
+      <c r="N37" t="s">
+        <v>172</v>
+      </c>
+      <c r="O37" t="s">
+        <v>181</v>
+      </c>
+      <c r="P37" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="19" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B38" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" t="s">
         <v>172</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="D38" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" t="s">
+        <v>187</v>
+      </c>
+      <c r="F38" t="s">
         <v>172</v>
       </c>
-      <c r="D38" s="16" t="s">
-        <v>172</v>
+      <c r="G38" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="B39" t="s">
-        <v>172</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>393</v>
-      </c>
-      <c r="B40" t="s">
-        <v>161</v>
-      </c>
-      <c r="C40" t="s">
-        <v>161</v>
-      </c>
-      <c r="D40" t="s">
-        <v>175</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="F40" t="s">
-        <v>172</v>
-      </c>
-      <c r="G40" t="s">
-        <v>172</v>
-      </c>
-      <c r="H40" t="s">
-        <v>172</v>
-      </c>
-      <c r="I40" t="s">
-        <v>161</v>
-      </c>
-      <c r="J40" t="s">
-        <v>180</v>
-      </c>
-      <c r="K40" t="s">
-        <v>180</v>
-      </c>
-      <c r="L40" t="s">
-        <v>180</v>
-      </c>
-      <c r="M40" t="s">
-        <v>180</v>
-      </c>
-      <c r="N40" t="s">
-        <v>172</v>
-      </c>
-      <c r="O40" t="s">
-        <v>181</v>
-      </c>
-      <c r="P40" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A41" s="19" t="s">
-        <v>394</v>
-      </c>
-      <c r="B41" t="s">
-        <v>161</v>
-      </c>
-      <c r="C41" t="s">
-        <v>172</v>
-      </c>
-      <c r="D41" t="s">
-        <v>175</v>
-      </c>
-      <c r="E41" t="s">
-        <v>187</v>
-      </c>
-      <c r="F41" t="s">
-        <v>172</v>
-      </c>
-      <c r="G41" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A42" s="19" t="s">
-        <v>384</v>
-      </c>
-      <c r="B42" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="19" t="s">
+    <row r="40" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="19" t="s">
         <v>385</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B40" s="19" t="s">
         <v>185</v>
       </c>
     </row>
@@ -5891,7 +5867,7 @@
   </sheetPr>
   <dimension ref="A1:AF66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X4" sqref="X4:Y4"/>
     </sheetView>
   </sheetViews>
@@ -6924,10 +6900,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7021,6 +6997,23 @@
         <v>412</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>401</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>271</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Fix database read issues. Fix TimeSeries plot.
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -1246,12 +1246,6 @@
     <t>filter.device_floating</t>
   </si>
   <si>
-    <t>power_factor_constant</t>
-  </si>
-  <si>
-    <t>power_factor_variable</t>
-  </si>
-  <si>
     <t>device.control_signal_cable</t>
   </si>
   <si>
@@ -1400,6 +1394,12 @@
   </si>
   <si>
     <t>centre_of_gravity</t>
+  </si>
+  <si>
+    <t>constant_power_factor</t>
+  </si>
+  <si>
+    <t>variable_power_factor</t>
   </si>
 </sst>
 </file>
@@ -2118,16 +2118,16 @@
     </row>
     <row r="7" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
@@ -2141,7 +2141,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
@@ -2333,7 +2333,7 @@
     </row>
     <row r="20" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>6</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="21" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>6</v>
@@ -2367,7 +2367,7 @@
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="36" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>6</v>
@@ -2376,7 +2376,7 @@
         <v>39</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
@@ -2513,7 +2513,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>300</v>
@@ -3251,7 +3251,7 @@
         <v>90</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>95</v>
@@ -3287,34 +3287,34 @@
         <v>93</v>
       </c>
       <c r="O4" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q4" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="P4" s="13" t="s">
+      <c r="R4" s="13" t="s">
         <v>431</v>
       </c>
-      <c r="Q4" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>433</v>
-      </c>
       <c r="S4" s="13" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="U4" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="V4" s="13" t="s">
         <v>91</v>
       </c>
       <c r="W4" s="19" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="X4" s="19" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="Y4" s="16" t="s">
         <v>103</v>
@@ -3374,37 +3374,37 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B6" t="s">
         <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D6" t="s">
         <v>114</v>
       </c>
       <c r="E6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I6" t="s">
         <v>106</v>
       </c>
       <c r="J6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="L6" t="s">
         <v>107</v>
@@ -3428,10 +3428,10 @@
         <v>113</v>
       </c>
       <c r="S6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="U6" s="16" t="s">
         <v>104</v>
@@ -3445,31 +3445,31 @@
         <v>90</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>114</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I7" s="19" t="s">
         <v>106</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="L7" s="19" t="s">
         <v>107</v>
@@ -3493,10 +3493,10 @@
         <v>113</v>
       </c>
       <c r="S7" s="19" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="T7" s="16" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="U7" s="16" t="s">
         <v>104</v>
@@ -3510,7 +3510,7 @@
         <v>90</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>95</v>
@@ -3531,28 +3531,28 @@
         <v>93</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="K8" s="19" t="s">
         <v>116</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="M8" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="O8" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="N8" s="13" t="s">
-        <v>443</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>444</v>
-      </c>
       <c r="P8" s="19" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="R8" s="19" t="s">
         <v>103</v>
@@ -3569,7 +3569,7 @@
         <v>90</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>95</v>
@@ -3593,31 +3593,31 @@
         <v>105</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="N9" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="O9" s="19" t="s">
         <v>91</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="R9" s="19" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S9" s="19" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="T9" s="19" t="s">
         <v>103</v>
@@ -3634,7 +3634,7 @@
         <v>90</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>95</v>
@@ -3658,31 +3658,31 @@
         <v>105</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="N10" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="O10" s="19" t="s">
         <v>91</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S10" s="19" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="T10" s="19" t="s">
         <v>103</v>
@@ -4145,7 +4145,7 @@
     </row>
     <row r="4" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>159</v>
@@ -4544,7 +4544,7 @@
     </row>
     <row r="17" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>162</v>
@@ -4552,7 +4552,7 @@
     </row>
     <row r="18" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>160</v>
@@ -4560,7 +4560,7 @@
     </row>
     <row r="19" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>159</v>
@@ -4957,7 +4957,7 @@
   </sheetPr>
   <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
@@ -5127,7 +5127,7 @@
         <v>176</v>
       </c>
       <c r="Y4" s="16" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="Z4" s="16" t="s">
         <v>161</v>
@@ -5139,7 +5139,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>161</v>
@@ -5151,10 +5151,10 @@
         <v>172</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>173</v>
@@ -5196,7 +5196,7 @@
         <v>174</v>
       </c>
       <c r="T5" s="16" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="U5" s="16" t="s">
         <v>161</v>
@@ -5226,10 +5226,10 @@
         <v>172</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G6" s="19" t="s">
         <v>173</v>
@@ -5271,7 +5271,7 @@
         <v>174</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="U6" s="16" t="s">
         <v>161</v>
@@ -5340,7 +5340,7 @@
         <v>174</v>
       </c>
       <c r="R7" s="16" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="S7" s="16" t="s">
         <v>161</v>
@@ -5406,7 +5406,7 @@
         <v>174</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="U8" s="16" t="s">
         <v>161</v>
@@ -5471,7 +5471,7 @@
         <v>174</v>
       </c>
       <c r="T9" s="16" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="U9" s="16" t="s">
         <v>161</v>
@@ -5717,7 +5717,7 @@
         <v>386</v>
       </c>
       <c r="B33" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -5867,8 +5867,8 @@
   </sheetPr>
   <dimension ref="A1:AF66"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4:Y4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5937,7 +5937,7 @@
         <v>193</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
@@ -5965,7 +5965,7 @@
         <v>193</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>200</v>
@@ -5995,10 +5995,10 @@
         <v>207</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="P4" s="16" t="s">
         <v>194</v>
@@ -6013,7 +6013,7 @@
         <v>197</v>
       </c>
       <c r="T4" s="19" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="U4" s="24" t="s">
         <v>230</v>
@@ -6053,7 +6053,7 @@
         <v>193</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E5" s="19" t="s">
         <v>200</v>
@@ -6068,16 +6068,16 @@
         <v>202</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>210</v>
       </c>
       <c r="L5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="M5" t="s">
         <v>213</v>
@@ -6092,10 +6092,10 @@
         <v>212</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="S5" t="s">
         <v>215</v>
@@ -6112,25 +6112,25 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B6" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>193</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>225</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H6" s="19" t="s">
         <v>227</v>
@@ -6142,7 +6142,7 @@
         <v>217</v>
       </c>
       <c r="K6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="L6" s="16" t="s">
         <v>211</v>
@@ -6172,7 +6172,7 @@
         <v>216</v>
       </c>
       <c r="U6" s="16" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="V6" s="16" t="s">
         <v>209</v>
@@ -6244,16 +6244,16 @@
         <v>193</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>225</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>227</v>
@@ -6265,7 +6265,7 @@
         <v>217</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="L8" s="16" t="s">
         <v>211</v>
@@ -6295,7 +6295,7 @@
         <v>216</v>
       </c>
       <c r="U8" s="16" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="V8" s="16" t="s">
         <v>209</v>
@@ -6312,7 +6312,7 @@
         <v>193</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>200</v>
@@ -6327,10 +6327,10 @@
         <v>202</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>229</v>
@@ -6376,7 +6376,7 @@
         <v>193</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>200</v>
@@ -6391,16 +6391,16 @@
         <v>202</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>210</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="M10" s="19" t="s">
         <v>213</v>
@@ -6415,10 +6415,10 @@
         <v>212</v>
       </c>
       <c r="Q10" s="16" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="R10" s="16" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="S10" s="19" t="s">
         <v>215</v>
@@ -6535,40 +6535,40 @@
         <v>402</v>
       </c>
       <c r="C19" t="s">
-        <v>404</v>
+        <v>454</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B20" t="s">
         <v>402</v>
       </c>
       <c r="C20" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B21" t="s">
         <v>402</v>
       </c>
       <c r="C21" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B22" t="s">
         <v>402</v>
       </c>
       <c r="C22" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.35">
@@ -6625,7 +6625,7 @@
         <v>402</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>405</v>
+        <v>455</v>
       </c>
       <c r="D25" s="19"/>
     </row>
@@ -6991,10 +6991,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fix database read issues and order of hydrodynamics module inputs.
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -715,9 +715,6 @@
     <t>soil_gc</t>
   </si>
   <si>
-    <t>system_draft</t>
-  </si>
-  <si>
     <t>surface_current_flow_velocity</t>
   </si>
   <si>
@@ -1181,6 +1178,9 @@
   </si>
   <si>
     <t>variable_power_factor</t>
+  </si>
+  <si>
+    <t>draft</t>
   </si>
 </sst>
 </file>
@@ -1791,10 +1791,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>306</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -1811,10 +1811,10 @@
         <v>67</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -1825,10 +1825,10 @@
         <v>65</v>
       </c>
       <c r="C3" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>283</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -1842,7 +1842,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -1856,7 +1856,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -1875,16 +1875,16 @@
     </row>
     <row r="7" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -1898,7 +1898,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -1912,7 +1912,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -1926,7 +1926,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1937,10 +1937,10 @@
         <v>25</v>
       </c>
       <c r="C11" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="D11" s="25" t="s">
         <v>250</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>251</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
@@ -1951,16 +1951,16 @@
     </row>
     <row r="12" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>293</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>294</v>
       </c>
       <c r="G12" s="24" t="s">
         <v>26</v>
@@ -1974,10 +1974,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>271</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>272</v>
       </c>
       <c r="G13" s="24" t="s">
         <v>26</v>
@@ -1991,10 +1991,10 @@
         <v>41</v>
       </c>
       <c r="C14" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>267</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>268</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
@@ -2011,10 +2011,10 @@
         <v>41</v>
       </c>
       <c r="C15" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>289</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>290</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
@@ -2031,10 +2031,10 @@
         <v>43</v>
       </c>
       <c r="C16" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>269</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>270</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
@@ -2074,7 +2074,7 @@
         <v>54</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
@@ -2091,10 +2091,10 @@
         <v>46</v>
       </c>
       <c r="C19" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="D19" s="25" t="s">
         <v>275</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>276</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
@@ -2111,10 +2111,10 @@
         <v>6</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
@@ -2134,7 +2134,7 @@
         <v>49</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G21" s="24" t="s">
         <v>7</v>
@@ -2148,10 +2148,10 @@
         <v>6</v>
       </c>
       <c r="C22" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="D22" s="25" t="s">
         <v>279</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>280</v>
       </c>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
@@ -2171,7 +2171,7 @@
         <v>51</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -2182,16 +2182,16 @@
     </row>
     <row r="24" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="D24" s="27" t="s">
         <v>299</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>300</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
@@ -2200,13 +2200,13 @@
     </row>
     <row r="25" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="30" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>28</v>
@@ -2218,30 +2218,30 @@
     </row>
     <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>264</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>257</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="28" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>34</v>
@@ -2259,7 +2259,7 @@
         <v>35</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="29" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>34</v>
@@ -2277,7 +2277,7 @@
         <v>36</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="30" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>32</v>
@@ -2295,7 +2295,7 @@
         <v>33</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -2304,16 +2304,16 @@
     </row>
     <row r="31" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B31" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="D31" s="27" t="s">
         <v>303</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>304</v>
       </c>
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
@@ -2322,16 +2322,16 @@
     </row>
     <row r="32" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>245</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -2340,16 +2340,16 @@
     </row>
     <row r="33" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>252</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>253</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2358,16 +2358,16 @@
     </row>
     <row r="34" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>249</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="35" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>8</v>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="36" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>8</v>
@@ -2403,7 +2403,7 @@
         <v>31</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -2412,16 +2412,16 @@
     </row>
     <row r="37" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="30" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B37" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="D37" s="27" t="s">
         <v>301</v>
-      </c>
-      <c r="D37" s="27" t="s">
-        <v>302</v>
       </c>
       <c r="E37" s="26"/>
       <c r="F37" s="26"/>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="38" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>58</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>61</v>
@@ -2463,7 +2463,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>55</v>
@@ -2481,7 +2481,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>34</v>
@@ -2490,7 +2490,7 @@
         <v>11</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -2499,16 +2499,16 @@
     </row>
     <row r="42" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>259</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -2519,16 +2519,16 @@
     </row>
     <row r="43" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C43" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D43" s="20" t="s">
         <v>273</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>274</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -2537,16 +2537,16 @@
     </row>
     <row r="44" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D44" s="21" t="s">
         <v>277</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>278</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
@@ -2555,16 +2555,16 @@
     </row>
     <row r="45" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C45" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D45" s="22" t="s">
         <v>287</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>288</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
@@ -2699,7 +2699,7 @@
         <v>73</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>78</v>
@@ -2735,34 +2735,34 @@
         <v>76</v>
       </c>
       <c r="O4" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="P4" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="P4" s="13" t="s">
+      <c r="Q4" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="R4" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="R4" s="13" t="s">
-        <v>358</v>
-      </c>
       <c r="S4" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="T4" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="U4" s="13" t="s">
         <v>367</v>
-      </c>
-      <c r="U4" s="13" t="s">
-        <v>368</v>
       </c>
       <c r="V4" s="13" t="s">
         <v>74</v>
       </c>
       <c r="W4" s="18" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="X4" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Y4" s="16" t="s">
         <v>86</v>
@@ -2822,37 +2822,37 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B6" t="s">
         <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D6" t="s">
         <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G6" t="s">
+        <v>374</v>
+      </c>
+      <c r="H6" t="s">
         <v>375</v>
-      </c>
-      <c r="H6" t="s">
-        <v>376</v>
       </c>
       <c r="I6" t="s">
         <v>89</v>
       </c>
       <c r="J6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L6" t="s">
         <v>90</v>
@@ -2876,10 +2876,10 @@
         <v>96</v>
       </c>
       <c r="S6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="U6" s="16" t="s">
         <v>87</v>
@@ -2893,31 +2893,31 @@
         <v>73</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>97</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G7" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>375</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>376</v>
       </c>
       <c r="I7" s="18" t="s">
         <v>89</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L7" s="18" t="s">
         <v>90</v>
@@ -2941,10 +2941,10 @@
         <v>96</v>
       </c>
       <c r="S7" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="T7" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="U7" s="16" t="s">
         <v>87</v>
@@ -2958,7 +2958,7 @@
         <v>73</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>78</v>
@@ -2979,28 +2979,28 @@
         <v>76</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K8" s="18" t="s">
         <v>98</v>
       </c>
       <c r="L8" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q8" s="18" t="s">
         <v>371</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>367</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>369</v>
-      </c>
-      <c r="P8" s="18" t="s">
-        <v>374</v>
-      </c>
-      <c r="Q8" s="18" t="s">
-        <v>372</v>
       </c>
       <c r="R8" s="18" t="s">
         <v>86</v>
@@ -3017,7 +3017,7 @@
         <v>73</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>78</v>
@@ -3041,31 +3041,31 @@
         <v>88</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L9" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="M9" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="M9" s="18" t="s">
-        <v>362</v>
-      </c>
       <c r="N9" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O9" s="18" t="s">
         <v>74</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Q9" s="18" t="s">
+        <v>372</v>
+      </c>
+      <c r="R9" s="18" t="s">
         <v>373</v>
       </c>
-      <c r="R9" s="18" t="s">
-        <v>374</v>
-      </c>
       <c r="S9" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="T9" s="18" t="s">
         <v>86</v>
@@ -3082,7 +3082,7 @@
         <v>73</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>78</v>
@@ -3106,31 +3106,31 @@
         <v>88</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L10" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="M10" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="M10" s="18" t="s">
-        <v>362</v>
-      </c>
       <c r="N10" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O10" s="18" t="s">
         <v>74</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Q10" s="18" t="s">
+        <v>372</v>
+      </c>
+      <c r="R10" s="18" t="s">
         <v>373</v>
       </c>
-      <c r="R10" s="18" t="s">
-        <v>374</v>
-      </c>
       <c r="S10" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="T10" s="18" t="s">
         <v>86</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B12" t="s">
         <v>73</v>
@@ -3173,7 +3173,7 @@
         <v>79</v>
       </c>
       <c r="H12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I12" t="s">
         <v>105</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B13" t="s">
         <v>73</v>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B14" t="s">
         <v>73</v>
@@ -3230,7 +3230,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B15" t="s">
         <v>109</v>
@@ -3280,7 +3280,7 @@
     </row>
     <row r="16" spans="1:32" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>73</v>
@@ -3379,7 +3379,7 @@
   </sheetPr>
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
@@ -3554,7 +3554,7 @@
     </row>
     <row r="4" spans="1:31" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>137</v>
@@ -3883,7 +3883,7 @@
     </row>
     <row r="9" spans="1:31" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>137</v>
@@ -3955,7 +3955,7 @@
     </row>
     <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>137</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>136</v>
@@ -3971,7 +3971,7 @@
     </row>
     <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>141</v>
@@ -4000,7 +4000,7 @@
     </row>
     <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>138</v>
@@ -4008,7 +4008,7 @@
     </row>
     <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>136</v>
@@ -4025,7 +4025,7 @@
     </row>
     <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>136</v>
@@ -4033,7 +4033,7 @@
     </row>
     <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>136</v>
@@ -4041,7 +4041,7 @@
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>136</v>
@@ -4049,7 +4049,7 @@
     </row>
     <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>136</v>
@@ -4057,7 +4057,7 @@
     </row>
     <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>137</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>136</v>
@@ -4073,7 +4073,7 @@
     </row>
     <row r="29" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>137</v>
@@ -4081,7 +4081,7 @@
     </row>
     <row r="30" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>137</v>
@@ -4131,7 +4131,7 @@
     </row>
     <row r="31" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>136</v>
@@ -4139,7 +4139,7 @@
     </row>
     <row r="32" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>137</v>
@@ -4162,7 +4162,7 @@
     </row>
     <row r="33" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>136</v>
@@ -4356,7 +4356,7 @@
         <v>154</v>
       </c>
       <c r="Y4" s="16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="Z4" s="16" t="s">
         <v>139</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>139</v>
@@ -4380,10 +4380,10 @@
         <v>150</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>151</v>
@@ -4425,7 +4425,7 @@
         <v>152</v>
       </c>
       <c r="T5" s="16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="U5" s="16" t="s">
         <v>139</v>
@@ -4455,10 +4455,10 @@
         <v>150</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>151</v>
@@ -4500,7 +4500,7 @@
         <v>152</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="U6" s="16" t="s">
         <v>139</v>
@@ -4569,7 +4569,7 @@
         <v>152</v>
       </c>
       <c r="R7" s="16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S7" s="16" t="s">
         <v>139</v>
@@ -4635,7 +4635,7 @@
         <v>152</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="U8" s="16" t="s">
         <v>139</v>
@@ -4700,7 +4700,7 @@
         <v>152</v>
       </c>
       <c r="T9" s="16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="U9" s="16" t="s">
         <v>139</v>
@@ -4803,7 +4803,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B20" t="s">
         <v>139</v>
@@ -4832,7 +4832,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B21" t="s">
         <v>150</v>
@@ -4840,7 +4840,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B22" t="s">
         <v>146</v>
@@ -4848,17 +4848,17 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B23" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B24" t="s">
         <v>150</v>
@@ -4872,7 +4872,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B25" t="s">
         <v>150</v>
@@ -4886,7 +4886,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B26" t="s">
         <v>139</v>
@@ -4936,7 +4936,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B27" t="s">
         <v>139</v>
@@ -4975,8 +4975,8 @@
   </sheetPr>
   <dimension ref="A1:AF54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5039,13 +5039,13 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>169</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
@@ -5053,13 +5053,13 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>169</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
@@ -5067,13 +5067,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>169</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>176</v>
@@ -5103,10 +5103,10 @@
         <v>183</v>
       </c>
       <c r="N4" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="O4" s="16" t="s">
         <v>365</v>
-      </c>
-      <c r="O4" s="16" t="s">
-        <v>366</v>
       </c>
       <c r="P4" s="16" t="s">
         <v>170</v>
@@ -5121,7 +5121,7 @@
         <v>173</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="U4" s="23" t="s">
         <v>206</v>
@@ -5155,13 +5155,13 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>169</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>176</v>
@@ -5176,16 +5176,16 @@
         <v>178</v>
       </c>
       <c r="I5" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="J5" s="16" t="s">
         <v>365</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>366</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>186</v>
       </c>
       <c r="L5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M5" t="s">
         <v>189</v>
@@ -5200,10 +5200,10 @@
         <v>188</v>
       </c>
       <c r="Q5" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="R5" s="16" t="s">
         <v>363</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>364</v>
       </c>
       <c r="S5" t="s">
         <v>191</v>
@@ -5220,25 +5220,25 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>169</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>201</v>
       </c>
       <c r="F6" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>339</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>340</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>203</v>
@@ -5250,7 +5250,7 @@
         <v>193</v>
       </c>
       <c r="K6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L6" s="16" t="s">
         <v>187</v>
@@ -5280,7 +5280,7 @@
         <v>192</v>
       </c>
       <c r="U6" s="16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="V6" s="16" t="s">
         <v>185</v>
@@ -5292,7 +5292,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>214</v>
@@ -5346,22 +5346,22 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>169</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>201</v>
       </c>
       <c r="F8" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>339</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>340</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>203</v>
@@ -5373,7 +5373,7 @@
         <v>193</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L8" s="16" t="s">
         <v>187</v>
@@ -5403,7 +5403,7 @@
         <v>192</v>
       </c>
       <c r="U8" s="16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="V8" s="16" t="s">
         <v>185</v>
@@ -5414,13 +5414,13 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>169</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>176</v>
@@ -5435,10 +5435,10 @@
         <v>178</v>
       </c>
       <c r="I9" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>365</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>366</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>205</v>
@@ -5478,13 +5478,13 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>169</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>176</v>
@@ -5499,16 +5499,16 @@
         <v>178</v>
       </c>
       <c r="I10" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="J10" s="16" t="s">
         <v>365</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>366</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>186</v>
       </c>
       <c r="L10" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M10" s="18" t="s">
         <v>189</v>
@@ -5523,10 +5523,10 @@
         <v>188</v>
       </c>
       <c r="Q10" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="R10" s="16" t="s">
         <v>363</v>
-      </c>
-      <c r="R10" s="16" t="s">
-        <v>364</v>
       </c>
       <c r="S10" s="18" t="s">
         <v>191</v>
@@ -5546,21 +5546,21 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.35">
@@ -5568,10 +5568,10 @@
         <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.35">
@@ -5579,10 +5579,10 @@
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -5599,10 +5599,10 @@
         <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
@@ -5625,10 +5625,10 @@
         <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D16" s="18"/>
     </row>
@@ -5637,7 +5637,7 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>212</v>
@@ -5649,10 +5649,10 @@
         <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>227</v>
+        <v>382</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
@@ -5669,7 +5669,7 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>213</v>
@@ -5689,7 +5689,7 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>187</v>
@@ -5705,7 +5705,7 @@
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>210</v>
@@ -5726,10 +5726,10 @@
         <v>47</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:22" s="18" customFormat="1" x14ac:dyDescent="0.35">
@@ -5737,7 +5737,7 @@
         <v>50</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>211</v>
@@ -5868,27 +5868,27 @@
         <v>131</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>234</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" t="s">
         <v>236</v>
-      </c>
-      <c r="C2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -5896,63 +5896,63 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" t="s">
         <v>238</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>239</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>240</v>
-      </c>
-      <c r="E3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B4" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>296</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>297</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B5" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="E5" s="18" t="s">
         <v>240</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>240</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add labels and units to PointDict variables in DDSs
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8140" tabRatio="392" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="385">
   <si>
     <t>Identifier</t>
   </si>
@@ -1181,6 +1181,12 @@
   </si>
   <si>
     <t>draft</t>
+  </si>
+  <si>
+    <t>UTM x</t>
+  </si>
+  <si>
+    <t>UTM y</t>
   </si>
 </sst>
 </file>
@@ -1759,9 +1765,9 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A25" sqref="A25:XFD25"/>
+      <selection pane="topRight" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2591,7 +2597,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A15" sqref="A15:XFD15"/>
+      <selection pane="topRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3301,49 +3307,68 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B18" s="18"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>330</v>
+      </c>
+      <c r="B17" t="s">
+        <v>383</v>
+      </c>
+      <c r="C17" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>333</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" s="18"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B20" s="18"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B21" s="18"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B22" s="18"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B23" s="18"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B24" s="18"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B25" s="18"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B26" s="18"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B27" s="18"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B28" s="18"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B29" s="18"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B30" s="18"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" s="18"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" s="18"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
@@ -4184,10 +4209,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:AE27"/>
+  <dimension ref="A1:AE29"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4957,6 +4982,28 @@
         <v>139</v>
       </c>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="B28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AE1">
     <sortState ref="A2:AE45">
@@ -4975,7 +5022,7 @@
   </sheetPr>
   <dimension ref="A1:AF54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Set Star network layout as experimental
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FFDC55-3464-4CF2-BCE7-A70C7C061089}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3043C8F1-1F05-432E-9FF0-C91BF5F43B96}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Units" sheetId="4" r:id="rId4"/>
     <sheet name="Valid Values" sheetId="5" r:id="rId5"/>
     <sheet name="Tables" sheetId="6" r:id="rId6"/>
+    <sheet name="Experimental" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">Labels!$A$1:$AF$1</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="386">
   <si>
     <t>Identifier</t>
   </si>
@@ -1193,6 +1194,9 @@
   </si>
   <si>
     <t>Bill of materials for electrical network.</t>
+  </si>
+  <si>
+    <t>4…</t>
   </si>
 </sst>
 </file>
@@ -1742,9 +1746,9 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D29" sqref="C2:D45"/>
+      <selection pane="topRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2569,7 +2573,7 @@
   </sheetPr>
   <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="K6" sqref="K6"/>
@@ -4902,7 +4906,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5019,7 +5023,7 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5793,4 +5797,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D25A888-82B9-44FE-AD29-AD42C3C1FB5C}">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="20">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20">
+        <v>3</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Assign types to DataTable structures using the types metadata.
Fix compatibility issues with database keys in installation and maintenance data preparation.
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3043C8F1-1F05-432E-9FF0-C91BF5F43B96}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C814F08C-0FA2-4BB0-9C68-00DB958887B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="386">
   <si>
     <t>Identifier</t>
   </si>
@@ -1746,7 +1746,7 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A24" sqref="A24"/>
     </sheetView>
@@ -2574,9 +2574,9 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="K6" sqref="K6"/>
+      <selection pane="topRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3320,10 +3320,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:AE33"/>
+  <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3938,7 +3938,7 @@
         <v>249</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4069,7 +4069,7 @@
         <v>250</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4103,12 +4103,35 @@
         <v>248</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>250</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" t="s">
+        <v>249</v>
+      </c>
+      <c r="C34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D34" t="s">
+        <v>250</v>
+      </c>
+      <c r="E34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F34" t="s">
+        <v>250</v>
+      </c>
+      <c r="G34" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -5806,7 +5829,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ensure component ids are always entered as strings
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C814F08C-0FA2-4BB0-9C68-00DB958887B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876B16C8-0DB3-4AF6-8818-8A8AB9BF8AB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="386">
   <si>
     <t>Identifier</t>
   </si>
@@ -1310,7 +1310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1358,6 +1358,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1746,9 +1750,9 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A24" sqref="A24"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2574,7 +2578,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="G16" sqref="G16"/>
     </sheetView>
@@ -3320,10 +3324,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:AE34"/>
+  <dimension ref="A1:AE36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3371,133 +3375,73 @@
       <c r="Y1" s="24"/>
       <c r="Z1" s="24"/>
     </row>
-    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
+    <row r="2" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+    </row>
+    <row r="3" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>250</v>
-      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
     </row>
     <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>249</v>
@@ -3521,64 +3465,69 @@
         <v>250</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>250</v>
-      </c>
       <c r="Q4" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>250</v>
       </c>
       <c r="U4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z4" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
     </row>
     <row r="5" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>249</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>250</v>
@@ -3596,10 +3545,10 @@
         <v>250</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>250</v>
@@ -3612,35 +3561,14 @@
       </c>
       <c r="N5" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>249</v>
@@ -3661,16 +3589,16 @@
         <v>250</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>250</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>250</v>
@@ -3691,15 +3619,31 @@
         <v>250</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>251</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
     </row>
     <row r="7" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>249</v>
@@ -3720,13 +3664,13 @@
         <v>250</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>248</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>250</v>
@@ -3756,15 +3700,15 @@
         <v>250</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>249</v>
@@ -3788,14 +3732,14 @@
         <v>250</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>250</v>
-      </c>
       <c r="M8" s="1" t="s">
         <v>250</v>
       </c>
@@ -3815,42 +3759,150 @@
         <v>250</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="U8" s="1" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>249</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="10" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>250</v>
@@ -3858,7 +3910,7 @@
     </row>
     <row r="13" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>250</v>
@@ -3866,7 +3918,7 @@
     </row>
     <row r="14" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>250</v>
@@ -3874,7 +3926,7 @@
     </row>
     <row r="15" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>250</v>
@@ -3882,7 +3934,7 @@
     </row>
     <row r="16" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>250</v>
@@ -3890,7 +3942,7 @@
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>250</v>
@@ -3898,15 +3950,15 @@
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>250</v>
@@ -3914,77 +3966,77 @@
     </row>
     <row r="20" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="H20" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>248</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>250</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>250</v>
@@ -3992,7 +4044,7 @@
     </row>
     <row r="26" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>250</v>
@@ -4000,15 +4052,15 @@
     </row>
     <row r="27" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>250</v>
@@ -4016,7 +4068,7 @@
     </row>
     <row r="29" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>249</v>
@@ -4024,71 +4076,29 @@
     </row>
     <row r="30" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>249</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>250</v>
@@ -4100,37 +4110,95 @@
         <v>250</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="P32" s="1" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B35" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>98</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>249</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>249</v>
       </c>
-      <c r="D34" t="s">
-        <v>250</v>
-      </c>
-      <c r="E34" t="s">
-        <v>250</v>
-      </c>
-      <c r="F34" t="s">
-        <v>250</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="D36" t="s">
+        <v>250</v>
+      </c>
+      <c r="E36" t="s">
+        <v>250</v>
+      </c>
+      <c r="F36" t="s">
+        <v>250</v>
+      </c>
+      <c r="G36" t="s">
         <v>248</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix column type of key indentifier in electrical outputs
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876B16C8-0DB3-4AF6-8818-8A8AB9BF8AB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFD6DCA-BF45-44BB-BC1B-08A9251FC714}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="385">
   <si>
     <t>Identifier</t>
   </si>
@@ -795,9 +795,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float </t>
   </si>
   <si>
     <t>bool</t>
@@ -1750,7 +1747,7 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
@@ -1859,7 +1856,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>25</v>
@@ -2269,7 +2266,7 @@
         <v>102</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
@@ -2580,7 +2577,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="G16" sqref="G16"/>
+      <selection pane="topRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3326,8 +3323,8 @@
   </sheetPr>
   <dimension ref="A1:AE36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3985,13 +3982,13 @@
         <v>91</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>248</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>250</v>
@@ -4022,10 +4019,10 @@
         <v>101</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>250</v>
@@ -4232,16 +4229,16 @@
         <v>243</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>256</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4249,13 +4246,13 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -4296,37 +4293,37 @@
         <v>251</v>
       </c>
       <c r="D4" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="H4" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="I4" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="J4" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>258</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="N4" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>251</v>
@@ -4344,22 +4341,22 @@
         <v>251</v>
       </c>
       <c r="T4" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="W4" s="22" t="s">
+      <c r="X4" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="Y4" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="X4" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="Z4" s="1" t="s">
         <v>251</v>
@@ -4380,19 +4377,19 @@
         <v>251</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>251</v>
@@ -4401,34 +4398,34 @@
         <v>251</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>263</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O5" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>251</v>
@@ -4455,19 +4452,19 @@
         <v>251</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>251</v>
@@ -4476,34 +4473,34 @@
         <v>251</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>263</v>
-      </c>
       <c r="M6" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>251</v>
@@ -4530,49 +4527,49 @@
         <v>251</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>251</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P7" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>251</v>
@@ -4590,22 +4587,22 @@
         <v>251</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>251</v>
@@ -4614,31 +4611,31 @@
         <v>251</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N8" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>251</v>
@@ -4655,22 +4652,22 @@
         <v>251</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>251</v>
@@ -4679,31 +4676,31 @@
         <v>251</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N9" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="P9" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>251</v>
@@ -4714,7 +4711,7 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -4722,10 +4719,10 @@
         <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -4733,7 +4730,7 @@
         <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C12" t="s">
         <v>251</v>
@@ -4744,7 +4741,7 @@
         <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -4752,7 +4749,7 @@
         <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -4760,7 +4757,7 @@
         <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -4772,7 +4769,7 @@
         <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -4780,7 +4777,7 @@
         <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -4788,7 +4785,7 @@
         <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E18" s="1"/>
     </row>
@@ -4797,7 +4794,7 @@
         <v>81</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -4812,19 +4809,19 @@
         <v>251</v>
       </c>
       <c r="C20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D20" t="s">
         <v>251</v>
       </c>
       <c r="E20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H20" t="s">
         <v>251</v>
@@ -4838,7 +4835,7 @@
         <v>113</v>
       </c>
       <c r="B21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -4846,7 +4843,7 @@
         <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -4854,7 +4851,7 @@
         <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -4864,13 +4861,13 @@
         <v>128</v>
       </c>
       <c r="B24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -4878,13 +4875,13 @@
         <v>132</v>
       </c>
       <c r="B25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -4898,40 +4895,40 @@
         <v>251</v>
       </c>
       <c r="D26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I26" t="s">
         <v>251</v>
       </c>
       <c r="J26" t="s">
+        <v>258</v>
+      </c>
+      <c r="K26" t="s">
+        <v>258</v>
+      </c>
+      <c r="L26" t="s">
+        <v>258</v>
+      </c>
+      <c r="M26" t="s">
+        <v>258</v>
+      </c>
+      <c r="N26" t="s">
+        <v>257</v>
+      </c>
+      <c r="O26" t="s">
         <v>259</v>
-      </c>
-      <c r="K26" t="s">
-        <v>259</v>
-      </c>
-      <c r="L26" t="s">
-        <v>259</v>
-      </c>
-      <c r="M26" t="s">
-        <v>259</v>
-      </c>
-      <c r="N26" t="s">
-        <v>258</v>
-      </c>
-      <c r="O26" t="s">
-        <v>260</v>
       </c>
       <c r="P26" t="s">
         <v>251</v>
@@ -4945,16 +4942,16 @@
         <v>251</v>
       </c>
       <c r="C27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G27" t="s">
         <v>251</v>
@@ -4965,10 +4962,10 @@
         <v>136</v>
       </c>
       <c r="B28" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C28" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -4976,10 +4973,10 @@
         <v>151</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -5013,16 +5010,16 @@
         <v>243</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>282</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5030,10 +5027,10 @@
         <v>119</v>
       </c>
       <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" t="s">
         <v>284</v>
-      </c>
-      <c r="C2" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5041,16 +5038,16 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" t="s">
         <v>286</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>287</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>288</v>
-      </c>
-      <c r="E3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5058,10 +5055,10 @@
         <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>290</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>291</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -5071,16 +5068,16 @@
         <v>84</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -5088,16 +5085,16 @@
         <v>125</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -5158,16 +5155,16 @@
         <v>243</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>294</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>295</v>
       </c>
       <c r="F1" s="3"/>
     </row>
@@ -5176,13 +5173,13 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -5190,13 +5187,13 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="30" x14ac:dyDescent="0.25">
@@ -5204,82 +5201,82 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>323</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
@@ -5292,67 +5289,67 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" t="s">
+        <v>315</v>
+      </c>
+      <c r="M5" t="s">
         <v>325</v>
       </c>
-      <c r="L5" t="s">
-        <v>316</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="N5" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="R5" s="1" t="s">
-        <v>331</v>
-      </c>
       <c r="S5" t="s">
+        <v>319</v>
+      </c>
+      <c r="T5" t="s">
         <v>320</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
@@ -5360,67 +5357,67 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" t="s">
         <v>336</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" t="s">
+        <v>315</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="K6" t="s">
-        <v>316</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" t="s">
         <v>341</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>342</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>343</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>344</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
+        <v>320</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="T6" t="s">
-        <v>321</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>346</v>
-      </c>
       <c r="V6" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="W6" s="1"/>
     </row>
@@ -5429,46 +5426,46 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -5483,67 +5480,67 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="U8" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>346</v>
-      </c>
       <c r="V8" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -5551,61 +5548,61 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
+        <v>361</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>366</v>
-      </c>
       <c r="Q9" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>323</v>
       </c>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
@@ -5615,67 +5612,67 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="K10" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="R10" s="1" t="s">
-        <v>331</v>
-      </c>
       <c r="S10" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
@@ -5683,13 +5680,13 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
+        <v>367</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D11" t="s">
         <v>368</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D11" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
@@ -5697,10 +5694,10 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
+        <v>369</v>
+      </c>
+      <c r="C12" t="s">
         <v>370</v>
-      </c>
-      <c r="C12" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
@@ -5708,10 +5705,10 @@
         <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
@@ -5719,10 +5716,10 @@
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -5739,10 +5736,10 @@
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -5765,10 +5762,10 @@
         <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -5777,10 +5774,10 @@
         <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -5789,10 +5786,10 @@
         <v>65</v>
       </c>
       <c r="B18" t="s">
+        <v>375</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -5809,10 +5806,10 @@
         <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -5829,10 +5826,10 @@
         <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H20" s="1"/>
       <c r="J20" s="1"/>
@@ -5845,10 +5842,10 @@
         <v>75</v>
       </c>
       <c r="B21" t="s">
+        <v>378</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -5866,10 +5863,10 @@
         <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5877,10 +5874,10 @@
         <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -5920,7 +5917,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5928,7 +5925,7 @@
         <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add unit to maximum cable lay gradient
</commit_message>
<xml_diff>
--- a/dds/electrical.xlsx
+++ b/dds/electrical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFD6DCA-BF45-44BB-BC1B-08A9251FC714}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C41463-B996-4ACA-B6B1-82282661DEA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="385">
   <si>
     <t>Identifier</t>
   </si>
@@ -1747,9 +1747,9 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
+      <selection pane="topRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3323,7 +3323,7 @@
   </sheetPr>
   <dimension ref="A1:AE36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -4211,10 +4211,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:AE29"/>
+  <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4977,6 +4977,14 @@
       </c>
       <c r="C29" s="1" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>